<commit_message>
Split ECM titles into building name and ecm number for table searches
</commit_message>
<xml_diff>
--- a/Comparator.xlsx
+++ b/Comparator.xlsx
@@ -8,19 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coder\Desktop\WordExcelComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BAD9D1-BE9D-479A-9E0D-D477CFDB3E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584564F2-DFDD-4FC5-B00F-0B9BA23BE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+  <si>
+    <t>Instructions:  Copy the label for each data type as found in eProjectBuilder from the Volume 1 and 2 Word submittals into the yellow alias fields below.  The tables must be native Word or Excel tables, not pasted images.  Copy the .docx submittals into the project directory and rename them as Vol1.docx and Vol2.docx.  Copy the eProjectBuilder workbook into the project directory and rename it to epb.xlsx, and make sure this file is named Comparator.xlsx.  Make sure the directory contains docExtract.py and comparator.py.  Run comparator.py with Python 3, or a Python IDE such as PyCharm: https://www.jetbrains.com/pycharm/download</t>
+  </si>
+  <si>
+    <t>Note: Discrepancies will be highlighted RED</t>
+  </si>
+  <si>
+    <t>Only green alias is currently implemented</t>
+  </si>
   <si>
     <t>ePB Schedule 4 Savings Comparator</t>
   </si>
@@ -266,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +308,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +401,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -397,6 +429,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,11 +452,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -748,7 +790,7 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -770,65 +812,85 @@
     <col min="16" max="16" width="3.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1" spans="1:16" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="18"/>
+        <v>8</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -841,7 +903,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -849,48 +911,48 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="M6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="O6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="9">
         <v>1942029.96199376</v>
@@ -899,18 +961,18 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G7" s="7">
         <v>57171.01823675519</v>
       </c>
       <c r="H7" s="7">
-        <v>57171</v>
+        <v>57175</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="L7" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M7" s="13">
         <v>1942030.2642937601</v>
@@ -921,7 +983,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -933,7 +995,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="L8" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="2"/>
@@ -942,7 +1004,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="9">
         <v>38972</v>
@@ -968,7 +1030,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="9">
         <v>31552</v>
@@ -994,7 +1056,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="9">
         <v>11633</v>
@@ -1020,7 +1082,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="9">
         <v>1128.5</v>
@@ -1046,7 +1108,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B13" s="9">
         <v>32168</v>
@@ -1061,7 +1123,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="L13" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M13" s="13">
         <v>793536</v>
@@ -1072,7 +1134,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" s="9">
         <v>7593</v>
@@ -1086,6 +1148,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="3">
         <v>6.01</v>
       </c>
@@ -1098,7 +1161,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" s="9">
         <v>27239</v>
@@ -1124,7 +1187,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" s="9">
         <v>26392</v>
@@ -1150,7 +1213,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B17" s="9">
         <v>24466</v>
@@ -1176,7 +1239,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" s="9">
         <v>8529.2642937599994</v>
@@ -1197,7 +1260,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" s="9">
         <v>10727.64</v>
@@ -1218,7 +1281,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B20" s="9">
         <v>21949</v>
@@ -1239,7 +1302,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B21" s="9">
         <v>7695</v>
@@ -1260,7 +1323,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B22" s="9">
         <v>23282</v>
@@ -1281,7 +1344,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B23" s="9">
         <v>123694</v>
@@ -1302,7 +1365,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B24" s="9">
         <v>109685</v>
@@ -1323,7 +1386,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" s="9">
         <v>163856</v>
@@ -1344,7 +1407,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" s="9">
         <v>52438</v>
@@ -1365,7 +1428,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" s="9">
         <v>60219</v>
@@ -1386,7 +1449,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B28" s="9">
         <v>30350</v>
@@ -1407,7 +1470,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B29" s="9">
         <v>6126</v>
@@ -1428,7 +1491,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B30" s="9">
         <v>12614</v>
@@ -1449,7 +1512,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31" s="9">
         <v>16277</v>
@@ -1470,7 +1533,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B32" s="9">
         <v>6422</v>
@@ -1491,7 +1554,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B33" s="9">
         <v>96536</v>
@@ -1512,7 +1575,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B34" s="9">
         <v>39132</v>
@@ -1533,7 +1596,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B35" s="9">
         <v>1817.28</v>
@@ -1554,7 +1617,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B36" s="9">
         <v>50683</v>
@@ -1575,7 +1638,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B37" s="9">
         <v>21848</v>
@@ -1596,7 +1659,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B38" s="9">
         <v>1817.28</v>
@@ -1617,7 +1680,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B39" s="9">
         <v>99519</v>
@@ -1638,7 +1701,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B40" s="9">
         <v>16989</v>
@@ -1659,7 +1722,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B41" s="9">
         <v>36997</v>
@@ -1680,7 +1743,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B42" s="9">
         <v>45035</v>
@@ -1701,7 +1764,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B43" s="9">
         <v>70327</v>
@@ -1722,7 +1785,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B44" s="9">
         <v>62439</v>
@@ -1743,7 +1806,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B45" s="9">
         <v>26886</v>
@@ -1764,7 +1827,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B46" s="9">
         <v>30254</v>
@@ -1785,7 +1848,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B47" s="9">
         <v>73579</v>
@@ -1806,7 +1869,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B48" s="9">
         <v>32640</v>
@@ -1827,7 +1890,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B49" s="9">
         <v>14816</v>
@@ -1848,7 +1911,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B50" s="9">
         <v>89230.997700000007</v>
@@ -1869,7 +1932,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B51" s="9">
         <v>58047</v>
@@ -1890,7 +1953,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" s="9">
         <v>122667</v>
@@ -1911,7 +1974,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B53" s="9">
         <v>48008</v>
@@ -1932,7 +1995,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B54" s="9">
         <v>47755</v>
@@ -4808,7 +4871,9 @@
       <c r="P258" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="B2:C2"/>
@@ -4820,11 +4885,10 @@
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="H7:H258">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(NOT(ISBLANK($H7)), ROUND($H7, 0)&lt;&gt;ROUND($G7, 0))</formula>
+      <formula>AND(NOT(ISBLANK($H7)), ROUND($H7, 0) &lt;&gt; ROUND($G7, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ECM table functionality complete
</commit_message>
<xml_diff>
--- a/Comparator.xlsx
+++ b/Comparator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coder\Desktop\WordExcelComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584564F2-DFDD-4FC5-B00F-0B9BA23BE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D69EC-620D-4046-863D-229D82CF4C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12368" yWindow="0" windowWidth="14332" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparator" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Instructions:  Copy the label for each data type as found in eProjectBuilder from the Volume 1 and 2 Word submittals into the yellow alias fields below.  The tables must be native Word or Excel tables, not pasted images.  Copy the .docx submittals into the project directory and rename them as Vol1.docx and Vol2.docx.  Copy the eProjectBuilder workbook into the project directory and rename it to epb.xlsx, and make sure this file is named Comparator.xlsx.  Make sure the directory contains docExtract.py and comparator.py.  Run comparator.py with Python 3, or a Python IDE such as PyCharm: https://www.jetbrains.com/pycharm/download</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Note: Discrepancies will be highlighted RED</t>
   </si>
   <si>
-    <t>Only green alias is currently implemented</t>
-  </si>
-  <si>
     <t>ePB Schedule 4 Savings Comparator</t>
   </si>
   <si>
@@ -63,6 +60,12 @@
     <t>Annual Estimated Energy Savings (MMBtu)</t>
   </si>
   <si>
+    <t xml:space="preserve"> Total Utility ($/yr) Cost Savings Year 1 </t>
+  </si>
+  <si>
+    <t>Total Energy (mmBTU) Savings Year 1</t>
+  </si>
+  <si>
     <t>Table Alias for Vol. 2 (docx format)</t>
   </si>
   <si>
@@ -99,7 +102,7 @@
     <t>ECM Cost</t>
   </si>
   <si>
-    <t>RL TIMERLAKE  TC. 2.11</t>
+    <t>RL TIMBERLAKE TC. 2.11</t>
   </si>
   <si>
     <t>RL TIMBERLAKE TC. 5.01</t>
@@ -108,7 +111,7 @@
     <t>RL TIMBERLAKE TC. 12.01</t>
   </si>
   <si>
-    <t>RL TIMBERLAKE  TC.13.01</t>
+    <t>RL TIMBERLAKE TC.13.01</t>
   </si>
   <si>
     <t>ROGERS FED. TC.2.01</t>
@@ -135,13 +138,13 @@
     <t>ROGERS FED. TC.13.01</t>
   </si>
   <si>
-    <t>ROGERS AUTH TC.5.01</t>
-  </si>
-  <si>
-    <t>ROGERS AUTH TC.12.01</t>
-  </si>
-  <si>
-    <t>ROGERS AUTH TC.13.01</t>
+    <t>ROGERS AUT TC.5.01</t>
+  </si>
+  <si>
+    <t>ROGERS AUT TC.12.01</t>
+  </si>
+  <si>
+    <t>ROGERS AUT TC.13.01</t>
   </si>
   <si>
     <t>WD FERG. TC.2.01</t>
@@ -174,13 +177,13 @@
     <t>GAINESVILLE TC.13.01</t>
   </si>
   <si>
-    <t xml:space="preserve">              YOUNG A  TC.5.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               YOUNG A TC.12.01</t>
-  </si>
-  <si>
-    <t>YOUNG A  TC.13.01</t>
+    <t>YOUNG A TC.5.01</t>
+  </si>
+  <si>
+    <t>YOUNG A TC.12.01</t>
+  </si>
+  <si>
+    <t>YOUNG A TC.13.01</t>
   </si>
   <si>
     <t>YOUNG FED TC. 5.01</t>
@@ -228,7 +231,7 @@
     <t>SIMPSON TC.2.01</t>
   </si>
   <si>
-    <t>SIMPSON  C.3,01</t>
+    <t>SIMPSON  TC.3.01</t>
   </si>
   <si>
     <t xml:space="preserve"> SIMPSON TC.5.01</t>
@@ -286,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +317,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,7 +430,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -452,7 +449,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,7 +787,7 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,53 +826,55 @@
       <c r="L1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>2</v>
-      </c>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="21"/>
       <c r="D3" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
+      <c r="G3" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="J3" s="25"/>
       <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="21"/>
@@ -890,7 +889,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -903,7 +902,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -911,48 +910,48 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="9">
         <v>1942029.96199376</v>
@@ -961,18 +960,18 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7">
         <v>57171.01823675519</v>
       </c>
       <c r="H7" s="7">
-        <v>57175</v>
+        <v>57171</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="L7" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7" s="13">
         <v>1942030.2642937601</v>
@@ -983,7 +982,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -995,7 +994,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="L8" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="2"/>
@@ -1004,18 +1003,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9">
         <v>38972</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9">
+        <v>38972</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="G9" s="7">
         <v>1332.386</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11">
+        <v>1332</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="L9" s="3">
@@ -1030,18 +1033,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9">
         <v>31552</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9">
+        <v>31552</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="G10" s="7">
         <v>1015.47944</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11">
+        <v>1015</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="L10" s="3">
@@ -1056,18 +1063,22 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="9">
         <v>11633</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9">
+        <v>11633</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="G11" s="7">
         <v>397.71978000000001</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="11">
+        <v>398</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="L11" s="3">
@@ -1082,12 +1093,14 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="9">
         <v>1128.5</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9">
+        <v>1129</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="G12" s="7">
@@ -1108,22 +1121,26 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="9">
         <v>32168</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="9">
+        <v>32168</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="G13" s="7">
         <v>1178.9142400000001</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11">
+        <v>1179</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="L13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M13" s="13">
         <v>793536</v>
@@ -1134,18 +1151,22 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9">
         <v>7593</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9">
+        <v>7593</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="G14" s="7">
         <v>278.28271999999998</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11">
+        <v>278</v>
+      </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="15"/>
@@ -1161,18 +1182,22 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9">
         <v>27239</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9">
+        <v>27239</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="G15" s="7">
         <v>998.26248799999996</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="11">
+        <v>998</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="L15" s="3">
@@ -1187,18 +1212,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9">
         <v>26392</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9">
+        <v>26392</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="G16" s="7">
         <v>904.76686400000006</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="11">
+        <v>905</v>
+      </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="L16" s="3">
@@ -1213,18 +1242,22 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="9">
         <v>24466</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9">
+        <v>24466</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="G17" s="7">
         <v>896.67359999999996</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="11">
+        <v>897</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="L17" s="3">
@@ -1239,18 +1272,22 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="9">
         <v>8529.2642937599994</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="9">
+        <v>8529.26</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="G18" s="7">
         <v>312.58700075520011</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="11">
+        <v>313</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="M18" s="13"/>
@@ -1260,12 +1297,14 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="9">
         <v>10727.64</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9">
+        <v>23282</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="G19" s="7">
@@ -1281,18 +1320,22 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="9">
         <v>21949</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9">
+        <v>21949</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="G20" s="7">
         <v>775.44524000000001</v>
       </c>
-      <c r="H20" s="11"/>
+      <c r="H20" s="11">
+        <v>775</v>
+      </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="M20" s="13"/>
@@ -1302,18 +1345,22 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="9">
         <v>7695</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9">
+        <v>7695</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="G21" s="7">
         <v>270.39758799999998</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="11">
+        <v>270</v>
+      </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="M21" s="13"/>
@@ -1323,12 +1370,14 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="9">
         <v>23282</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9">
+        <v>10728</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="G22" s="7">
@@ -1344,18 +1393,22 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="9">
         <v>123694</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9">
+        <v>123694</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="G23" s="7">
         <v>4710.3376520000002</v>
       </c>
-      <c r="H23" s="11"/>
+      <c r="H23" s="11">
+        <v>4710</v>
+      </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="M23" s="13"/>
@@ -1365,18 +1418,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" s="9">
         <v>109685</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9">
+        <v>109685</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="G24" s="7">
         <v>4176.7861519999997</v>
       </c>
-      <c r="H24" s="11"/>
+      <c r="H24" s="11">
+        <v>4177</v>
+      </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="M24" s="13"/>
@@ -1386,18 +1443,22 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" s="9">
         <v>163856</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9">
+        <v>163856</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="G25" s="7">
         <v>5733.9376519999996</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="11">
+        <v>5734</v>
+      </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="M25" s="13"/>
@@ -1407,18 +1468,22 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="9">
         <v>52438</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9">
+        <v>52438</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="G26" s="7">
         <v>1921.785116</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="11">
+        <v>1922</v>
+      </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="M26" s="13"/>
@@ -1428,12 +1493,14 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" s="9">
         <v>60219</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9">
+        <v>60219</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="G27" s="7">
@@ -1449,18 +1516,22 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" s="9">
         <v>30350</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="9">
+        <v>30350</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="G28" s="7">
         <v>591.94788000000005</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="11">
+        <v>592</v>
+      </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="M28" s="13"/>
@@ -1470,18 +1541,22 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" s="9">
         <v>6126</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="9">
+        <v>6126</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="G29" s="7">
         <v>204.54939999999999</v>
       </c>
-      <c r="H29" s="11"/>
+      <c r="H29" s="11">
+        <v>205</v>
+      </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="M29" s="13"/>
@@ -1491,18 +1566,22 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="9">
         <v>12614</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="9">
+        <v>12614</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="G30" s="7">
         <v>421.12268799999998</v>
       </c>
-      <c r="H30" s="11"/>
+      <c r="H30" s="11">
+        <v>421</v>
+      </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="M30" s="13"/>
@@ -1512,18 +1591,22 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="9">
         <v>16277</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="9">
+        <v>16277</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="G31" s="7">
         <v>331.574748</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="11">
+        <v>332</v>
+      </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="M31" s="13"/>
@@ -1533,12 +1616,14 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="9">
         <v>6422</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="9">
+        <v>6422</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="G32" s="7">
@@ -1554,18 +1639,22 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="9">
         <v>96536</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="9">
+        <v>96536</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="G33" s="7">
         <v>3025.5909999999999</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="11">
+        <v>3026</v>
+      </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="M33" s="13"/>
@@ -1575,18 +1664,22 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" s="9">
         <v>39132</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="9">
+        <v>39132</v>
+      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="G34" s="7">
         <v>1306.458212</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="11">
+        <v>1306</v>
+      </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="M34" s="13"/>
@@ -1596,12 +1689,14 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B35" s="9">
         <v>1817.28</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="9">
+        <v>1817</v>
+      </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="G35" s="7">
@@ -1617,18 +1712,22 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" s="9">
         <v>50683</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="9">
+        <v>50683</v>
+      </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="G36" s="7">
         <v>1724.73188</v>
       </c>
-      <c r="H36" s="11"/>
+      <c r="H36" s="11">
+        <v>1725</v>
+      </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="M36" s="13"/>
@@ -1638,18 +1737,22 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B37" s="9">
         <v>21848</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9">
+        <v>21848</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="G37" s="7">
         <v>767.7</v>
       </c>
-      <c r="H37" s="11"/>
+      <c r="H37" s="11">
+        <v>768</v>
+      </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="M37" s="13"/>
@@ -1659,12 +1762,14 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B38" s="9">
         <v>1817.28</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="9">
+        <v>1817</v>
+      </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="G38" s="7">
@@ -1680,18 +1785,22 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B39" s="9">
         <v>99519</v>
       </c>
-      <c r="C39" s="9"/>
+      <c r="C39" s="9">
+        <v>99519</v>
+      </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="G39" s="7">
         <v>3409.7822000000001</v>
       </c>
-      <c r="H39" s="11"/>
+      <c r="H39" s="11">
+        <v>3410</v>
+      </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="M39" s="13"/>
@@ -1701,18 +1810,22 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B40" s="9">
         <v>16989</v>
       </c>
-      <c r="C40" s="9"/>
+      <c r="C40" s="9">
+        <v>16989</v>
+      </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="G40" s="7">
         <v>616.02636399999994</v>
       </c>
-      <c r="H40" s="11"/>
+      <c r="H40" s="11">
+        <v>616</v>
+      </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="M40" s="13"/>
@@ -1722,18 +1835,22 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" s="9">
         <v>36997</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="9">
+        <v>36997</v>
+      </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="G41" s="7">
         <v>1341.4789800000001</v>
       </c>
-      <c r="H41" s="11"/>
+      <c r="H41" s="11">
+        <v>1341</v>
+      </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="M41" s="13"/>
@@ -1743,12 +1860,14 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B42" s="9">
         <v>45035</v>
       </c>
-      <c r="C42" s="9"/>
+      <c r="C42" s="9">
+        <v>45035</v>
+      </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="G42" s="7">
@@ -1764,18 +1883,22 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B43" s="9">
         <v>70327</v>
       </c>
-      <c r="C43" s="9"/>
+      <c r="C43" s="9">
+        <v>70327</v>
+      </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="G43" s="7">
         <v>2525.9036000000001</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="11">
+        <v>2526</v>
+      </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="M43" s="13"/>
@@ -1785,18 +1908,22 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B44" s="9">
         <v>62439</v>
       </c>
-      <c r="C44" s="9"/>
+      <c r="C44" s="9">
+        <v>62439</v>
+      </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="G44" s="7">
         <v>2298.16966</v>
       </c>
-      <c r="H44" s="11"/>
+      <c r="H44" s="11">
+        <v>2298</v>
+      </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="M44" s="13"/>
@@ -1806,18 +1933,22 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B45" s="9">
         <v>26886</v>
       </c>
-      <c r="C45" s="9"/>
+      <c r="C45" s="9">
+        <v>26886</v>
+      </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="G45" s="7">
         <v>989.60283200000003</v>
       </c>
-      <c r="H45" s="11"/>
+      <c r="H45" s="11">
+        <v>990</v>
+      </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="M45" s="13"/>
@@ -1827,12 +1958,14 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B46" s="9">
         <v>30254</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="9">
+        <v>30254</v>
+      </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="G46" s="7">
@@ -1848,18 +1981,22 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" s="9">
         <v>73579</v>
       </c>
-      <c r="C47" s="9"/>
+      <c r="C47" s="9">
+        <v>73579</v>
+      </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="G47" s="7">
         <v>2305.3519200000001</v>
       </c>
-      <c r="H47" s="11"/>
+      <c r="H47" s="11">
+        <v>2305</v>
+      </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="M47" s="13"/>
@@ -1869,18 +2006,22 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="9">
         <v>32640</v>
       </c>
-      <c r="C48" s="9"/>
+      <c r="C48" s="9">
+        <v>32640</v>
+      </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="G48" s="7">
         <v>1014.28524</v>
       </c>
-      <c r="H48" s="11"/>
+      <c r="H48" s="11">
+        <v>1014</v>
+      </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="M48" s="13"/>
@@ -1890,12 +2031,14 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" s="9">
         <v>14816</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="9">
+        <v>14816</v>
+      </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="G49" s="7">
@@ -1911,18 +2054,22 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B50" s="9">
         <v>89230.997700000007</v>
       </c>
-      <c r="C50" s="9"/>
+      <c r="C50" s="9">
+        <v>89231</v>
+      </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="G50" s="7">
         <v>2365.1984000000002</v>
       </c>
-      <c r="H50" s="11"/>
+      <c r="H50" s="11">
+        <v>2365</v>
+      </c>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="M50" s="13"/>
@@ -1932,18 +2079,22 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B51" s="9">
         <v>58047</v>
       </c>
-      <c r="C51" s="9"/>
+      <c r="C51" s="9">
+        <v>58047</v>
+      </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="G51" s="7">
         <v>1830.4527</v>
       </c>
-      <c r="H51" s="11"/>
+      <c r="H51" s="11">
+        <v>1830</v>
+      </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="M51" s="13"/>
@@ -1953,18 +2104,22 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B52" s="9">
         <v>122667</v>
       </c>
-      <c r="C52" s="9"/>
+      <c r="C52" s="9">
+        <v>122667</v>
+      </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="G52" s="7">
         <v>3683.4245999999998</v>
       </c>
-      <c r="H52" s="11"/>
+      <c r="H52" s="11">
+        <v>3683</v>
+      </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="M52" s="13"/>
@@ -1974,18 +2129,22 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B53" s="9">
         <v>48008</v>
       </c>
-      <c r="C53" s="9"/>
+      <c r="C53" s="9">
+        <v>48008</v>
+      </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="G53" s="7">
         <v>1513.9043999999999</v>
       </c>
-      <c r="H53" s="11"/>
+      <c r="H53" s="11">
+        <v>1514</v>
+      </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="M53" s="13"/>
@@ -1995,12 +2154,14 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B54" s="9">
         <v>47755</v>
       </c>
-      <c r="C54" s="9"/>
+      <c r="C54" s="9">
+        <v>47755</v>
+      </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="G54" s="7">
@@ -2015,11 +2176,15 @@
       <c r="P54" s="1"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B55" s="9"/>
+      <c r="B55" s="9">
+        <v>1942029.96199376</v>
+      </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
-      <c r="G55" s="7"/>
+      <c r="G55" s="7">
+        <v>57171.01823675519</v>
+      </c>
       <c r="H55" s="11"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -4873,22 +5038,22 @@
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="I3:K3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
-  <conditionalFormatting sqref="H7:H258">
+  <conditionalFormatting sqref="H7:H258 C9:C258">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(NOT(ISBLANK($H7)), ROUND($H7, 0) &lt;&gt; ROUND($G7, 0))</formula>
+      <formula>AND(NOT(ISBLANK(C7)), ROUND(C7, 0) &lt;&gt; ROUND(B7, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add project identifier imports
</commit_message>
<xml_diff>
--- a/Comparator.xlsx
+++ b/Comparator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coder\Desktop\WordExcelComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D69EC-620D-4046-863D-229D82CF4C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41ACB1B-2E8F-40D0-8960-379564F76069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12368" yWindow="0" windowWidth="14332" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="165" windowWidth="27450" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparator" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
-  <si>
-    <t>Instructions:  Copy the label for each data type as found in eProjectBuilder from the Volume 1 and 2 Word submittals into the yellow alias fields below.  The tables must be native Word or Excel tables, not pasted images.  Copy the .docx submittals into the project directory and rename them as Vol1.docx and Vol2.docx.  Copy the eProjectBuilder workbook into the project directory and rename it to epb.xlsx, and make sure this file is named Comparator.xlsx.  Make sure the directory contains docExtract.py and comparator.py.  Run comparator.py with Python 3, or a Python IDE such as PyCharm: https://www.jetbrains.com/pycharm/download</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>NDER 6 Region 4</t>
+  </si>
+  <si>
+    <t>ESPC Phase</t>
+  </si>
+  <si>
+    <t>ESCO Name</t>
+  </si>
+  <si>
+    <t>ABM</t>
+  </si>
+  <si>
+    <t>Volume 1 Submittal Date</t>
+  </si>
+  <si>
+    <t>Volume 2 Submittal Date</t>
+  </si>
+  <si>
+    <t>eProject Builder Submittal Date</t>
+  </si>
+  <si>
+    <t>Total Discrepancies Found</t>
   </si>
   <si>
     <t>Note: Discrepancies will be highlighted RED</t>
   </si>
   <si>
-    <t>ePB Schedule 4 Savings Comparator</t>
-  </si>
-  <si>
     <t>Estimated annual cost savings ($/yr) from AE258</t>
   </si>
   <si>
@@ -54,19 +75,19 @@
     <t>ECM energy savings from column Y</t>
   </si>
   <si>
-    <t>Table Alias for Vol. 1 (docx format)</t>
+    <t>Volume 1 Table Aliases</t>
   </si>
   <si>
     <t>Annual Estimated Energy Savings (MMBtu)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Total Utility ($/yr) Cost Savings Year 1 </t>
+    <t xml:space="preserve">Total Utility ($/yr) Cost Savings Year 1 </t>
   </si>
   <si>
     <t>Total Energy (mmBTU) Savings Year 1</t>
   </si>
   <si>
-    <t>Table Alias for Vol. 2 (docx format)</t>
+    <t>Volume 2 Table Aliases</t>
   </si>
   <si>
     <t>ECMs by Building</t>
@@ -93,10 +114,16 @@
     <t>ECM Savings Template</t>
   </si>
   <si>
+    <t>ROGERS FED. TC.3.01</t>
+  </si>
+  <si>
+    <t>Total Energy</t>
+  </si>
+  <si>
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Total Energy</t>
+    <t>ROGERS FED. TC.5.01</t>
   </si>
   <si>
     <t>ECM Cost</t>
@@ -123,12 +150,6 @@
     <t>ROGERS FED. TC.2.04</t>
   </si>
   <si>
-    <t>ROGERS FED. TC.3.01</t>
-  </si>
-  <si>
-    <t>ROGERS FED. TC.5.01</t>
-  </si>
-  <si>
     <t>ROGERS FED. TC.8.01</t>
   </si>
   <si>
@@ -241,6 +262,12 @@
   </si>
   <si>
     <t>SIMPSON TC.13.01</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Error per volume/data point</t>
   </si>
 </sst>
 </file>
@@ -359,15 +386,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -390,6 +408,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -398,14 +429,14 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -427,37 +458,41 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -784,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P258"/>
+  <dimension ref="A2:P266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -809,462 +844,295 @@
     <col min="16" max="16" width="3.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="17"/>
-    </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="21"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="32">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="32">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="32">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="17">
+        <f>SUM(C9,D9,G9,H9,N9,O9)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="20">
+        <f t="array" ref="C9">SUM(IF(ROUND(B15:B266,0)&lt;&gt;ROUND(C15:C266,0), 1, 0)) + COUNTBLANK(B15:B266) + COUNTIF(B15:B266, 0) - COUNTBLANK(C15:C266) - COUNTIF(C15:C266, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="array" ref="D9">SUM(IF(ROUND(B15:B266,0)&lt;&gt;ROUND(D15:D266,0), 1, 0)) + COUNTBLANK(B15:B266) + COUNTIF(B15:B266, 0) - COUNTBLANK(D15:D266) - COUNTIF(D15:D266, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="array" ref="H9">SUM(IF(ROUND(G15:G266,0)&lt;&gt;ROUND(H15:H266,0), 1, 0)) + COUNTBLANK(G15:G266) + COUNTIF(G15:G266, 0) - COUNTBLANK(H15:H266) - COUNTIF(H15:H266, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <f t="array" ref="I9">SUM(IF(ROUND(G15:G266,0)&lt;&gt;ROUND(I15:I266,0), 1, 0)) + COUNTBLANK(G15:G266) + COUNTIF(G15:G266, 0) - COUNTBLANK(I15:I266) - COUNTIF(I15:I266, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="19">
+        <f t="array" ref="N9">SUM(IF(ROUND(M15:M266,0)&lt;&gt;ROUND(N15:N266,0), 1, 0)) + COUNTBLANK(M15:M266) + COUNTIF(M15:M266, 0) - COUNTBLANK(N15:N266) - COUNTIF(N15:N266, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="17">
+        <f t="array" ref="O9">SUM(IF(ROUND(M15:M266,0)&lt;&gt;ROUND(O15:O266,0), 1, 0)) + COUNTBLANK(M15:M266) + COUNTIF(M15:M266, 0) - COUNTBLANK(O15:O266) - COUNTIF(O15:O266, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B10" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="21"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5" t="s">
+      <c r="H10" s="24"/>
+      <c r="I10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="31"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="31"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="9">
         <v>1942029.96199376</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7">
-        <v>57171.01823675519</v>
-      </c>
-      <c r="H7" s="7">
-        <v>57171</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="L7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="13">
-        <v>1942030.2642937601</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="L8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="9">
-        <v>38972</v>
-      </c>
-      <c r="C9" s="9">
-        <v>38972</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="G9" s="7">
-        <v>1332.386</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1332</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="L9" s="3">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="M9" s="13">
-        <v>245093</v>
-      </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="9">
-        <v>31552</v>
-      </c>
-      <c r="C10" s="9">
-        <v>31552</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="G10" s="7">
-        <v>1015.47944</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1015</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="L10" s="3">
-        <v>2.04</v>
-      </c>
-      <c r="M10" s="13">
-        <v>7593</v>
-      </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9">
-        <v>11633</v>
-      </c>
-      <c r="C11" s="9">
-        <v>11633</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="G11" s="7">
-        <v>397.71978000000001</v>
-      </c>
-      <c r="H11" s="11">
-        <v>398</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="L11" s="3">
-        <v>2.11</v>
-      </c>
-      <c r="M11" s="13">
-        <v>38972</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1128.5</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1129</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="G12" s="7">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="L12" s="3">
-        <v>3.01</v>
-      </c>
-      <c r="M12" s="13">
-        <v>194971</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="9">
-        <v>32168</v>
-      </c>
-      <c r="C13" s="9">
-        <v>32168</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="G13" s="7">
-        <v>1178.9142400000001</v>
-      </c>
-      <c r="H13" s="11">
-        <v>1179</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="L13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="13">
-        <v>793536</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="9">
-        <v>7593</v>
-      </c>
-      <c r="C14" s="9">
-        <v>7593</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="G14" s="7">
-        <v>278.28271999999998</v>
-      </c>
-      <c r="H14" s="11">
-        <v>278</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="3">
-        <v>6.01</v>
-      </c>
-      <c r="M14" s="13">
-        <v>12614</v>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="9">
-        <v>27239</v>
-      </c>
-      <c r="C15" s="9">
-        <v>27239</v>
-      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
+      <c r="F15" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="G15" s="7">
-        <v>998.26248799999996</v>
-      </c>
-      <c r="H15" s="11">
-        <v>998</v>
+        <v>57171.01823675519</v>
+      </c>
+      <c r="H15" s="7">
+        <v>57171</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="L15" s="3">
-        <v>8.01</v>
+      <c r="L15" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="M15" s="13">
-        <v>103894</v>
+        <v>1942030.2642937601</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="L16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9">
-        <v>26392</v>
-      </c>
-      <c r="C16" s="9">
-        <v>26392</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="G16" s="7">
-        <v>904.76686400000006</v>
-      </c>
-      <c r="H16" s="11">
-        <v>905</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="L16" s="3">
-        <v>12.01</v>
-      </c>
-      <c r="M16" s="13">
-        <v>302083.26429376</v>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="9">
-        <v>24466</v>
+        <v>38972</v>
       </c>
       <c r="C17" s="9">
-        <v>24466</v>
+        <v>38972</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="G17" s="7">
-        <v>896.67359999999996</v>
+        <v>1332.386</v>
       </c>
       <c r="H17" s="11">
-        <v>897</v>
+        <v>1332</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="L17" s="3">
-        <v>13.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="M17" s="13">
-        <v>243274</v>
+        <v>245093</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1275,22 +1143,27 @@
         <v>33</v>
       </c>
       <c r="B18" s="9">
-        <v>8529.2642937599994</v>
+        <v>31552</v>
       </c>
       <c r="C18" s="9">
-        <v>8529.26</v>
+        <v>31552</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="G18" s="7">
-        <v>312.58700075520011</v>
+        <v>1015.47944</v>
       </c>
       <c r="H18" s="11">
-        <v>313</v>
+        <v>1015</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="M18" s="13"/>
+      <c r="L18" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="M18" s="13">
+        <v>7593</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1300,20 +1173,27 @@
         <v>34</v>
       </c>
       <c r="B19" s="9">
-        <v>10727.64</v>
+        <v>11633</v>
       </c>
       <c r="C19" s="9">
-        <v>23282</v>
+        <v>11633</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="G19" s="7">
-        <v>0</v>
-      </c>
-      <c r="H19" s="11"/>
+        <v>397.71978000000001</v>
+      </c>
+      <c r="H19" s="11">
+        <v>398</v>
+      </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="M19" s="13"/>
+      <c r="L19" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="M19" s="13">
+        <v>38972</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1323,22 +1203,25 @@
         <v>35</v>
       </c>
       <c r="B20" s="9">
-        <v>21949</v>
+        <v>1128.5</v>
       </c>
       <c r="C20" s="9">
-        <v>21949</v>
+        <v>1129</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="G20" s="7">
-        <v>775.44524000000001</v>
-      </c>
-      <c r="H20" s="11">
-        <v>775</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H20" s="11"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="M20" s="13"/>
+      <c r="L20" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="M20" s="13">
+        <v>194971</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1348,141 +1231,169 @@
         <v>36</v>
       </c>
       <c r="B21" s="9">
-        <v>7695</v>
+        <v>32168</v>
       </c>
       <c r="C21" s="9">
-        <v>7695</v>
+        <v>32168</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="G21" s="7">
-        <v>270.39758799999998</v>
+        <v>1178.9142400000001</v>
       </c>
       <c r="H21" s="11">
-        <v>270</v>
+        <v>1179</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="M21" s="13"/>
+      <c r="L21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" s="13">
+        <v>793536</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="9">
-        <v>23282</v>
+        <v>7593</v>
       </c>
       <c r="C22" s="9">
-        <v>10728</v>
+        <v>7593</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="G22" s="7">
-        <v>0</v>
-      </c>
-      <c r="H22" s="11"/>
+        <v>278.28271999999998</v>
+      </c>
+      <c r="H22" s="11">
+        <v>278</v>
+      </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
-      <c r="M22" s="13"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="3">
+        <v>6.01</v>
+      </c>
+      <c r="M22" s="13">
+        <v>12614</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>123694</v>
+        <v>27239</v>
       </c>
       <c r="C23" s="9">
-        <v>123694</v>
+        <v>27239</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="G23" s="7">
-        <v>4710.3376520000002</v>
+        <v>998.26248799999996</v>
       </c>
       <c r="H23" s="11">
-        <v>4710</v>
+        <v>998</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="M23" s="13"/>
+      <c r="L23" s="3">
+        <v>8.01</v>
+      </c>
+      <c r="M23" s="13">
+        <v>103894</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B24" s="9">
-        <v>109685</v>
+        <v>26392</v>
       </c>
       <c r="C24" s="9">
-        <v>109685</v>
+        <v>26392</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="G24" s="7">
-        <v>4176.7861519999997</v>
+        <v>904.76686400000006</v>
       </c>
       <c r="H24" s="11">
-        <v>4177</v>
+        <v>905</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="M24" s="13"/>
+      <c r="L24" s="3">
+        <v>12.01</v>
+      </c>
+      <c r="M24" s="13">
+        <v>302083.26429376</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="9">
-        <v>163856</v>
+        <v>24466</v>
       </c>
       <c r="C25" s="9">
-        <v>163856</v>
+        <v>24466</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="G25" s="7">
-        <v>5733.9376519999996</v>
+        <v>896.67359999999996</v>
       </c>
       <c r="H25" s="11">
-        <v>5734</v>
+        <v>897</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="M25" s="13"/>
+      <c r="L25" s="3">
+        <v>13.01</v>
+      </c>
+      <c r="M25" s="13">
+        <v>243274</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="9">
-        <v>52438</v>
+        <v>8529.2642937599994</v>
       </c>
       <c r="C26" s="9">
-        <v>52438</v>
+        <v>8529.26</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="G26" s="7">
-        <v>1921.785116</v>
+        <v>312.58700075520011</v>
       </c>
       <c r="H26" s="11">
-        <v>1922</v>
+        <v>313</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1493,13 +1404,13 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="9">
-        <v>60219</v>
+        <v>10727.64</v>
       </c>
       <c r="C27" s="9">
-        <v>60219</v>
+        <v>23282</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1516,21 +1427,21 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="9">
-        <v>30350</v>
+        <v>21949</v>
       </c>
       <c r="C28" s="9">
-        <v>30350</v>
+        <v>21949</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="G28" s="7">
-        <v>591.94788000000005</v>
+        <v>775.44524000000001</v>
       </c>
       <c r="H28" s="11">
-        <v>592</v>
+        <v>775</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -1541,21 +1452,21 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="9">
-        <v>6126</v>
+        <v>7695</v>
       </c>
       <c r="C29" s="9">
-        <v>6126</v>
+        <v>7695</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="G29" s="7">
-        <v>204.54939999999999</v>
+        <v>270.39758799999998</v>
       </c>
       <c r="H29" s="11">
-        <v>205</v>
+        <v>270</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -1566,22 +1477,20 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="9">
-        <v>12614</v>
+        <v>23282</v>
       </c>
       <c r="C30" s="9">
-        <v>12614</v>
+        <v>10728</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="G30" s="7">
-        <v>421.12268799999998</v>
-      </c>
-      <c r="H30" s="11">
-        <v>421</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H30" s="11"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="M30" s="13"/>
@@ -1591,21 +1500,21 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="9">
-        <v>16277</v>
+        <v>123694</v>
       </c>
       <c r="C31" s="9">
-        <v>16277</v>
+        <v>123694</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="G31" s="7">
-        <v>331.574748</v>
+        <v>4710.3376520000002</v>
       </c>
       <c r="H31" s="11">
-        <v>332</v>
+        <v>4710</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -1616,20 +1525,22 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="9">
-        <v>6422</v>
+        <v>109685</v>
       </c>
       <c r="C32" s="9">
-        <v>6422</v>
+        <v>109685</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="G32" s="7">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11"/>
+        <v>4176.7861519999997</v>
+      </c>
+      <c r="H32" s="11">
+        <v>4177</v>
+      </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="M32" s="13"/>
@@ -1639,21 +1550,21 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="9">
-        <v>96536</v>
+        <v>163856</v>
       </c>
       <c r="C33" s="9">
-        <v>96536</v>
+        <v>163856</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="G33" s="7">
-        <v>3025.5909999999999</v>
+        <v>5733.9376519999996</v>
       </c>
       <c r="H33" s="11">
-        <v>3026</v>
+        <v>5734</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -1664,21 +1575,21 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="9">
-        <v>39132</v>
+        <v>52438</v>
       </c>
       <c r="C34" s="9">
-        <v>39132</v>
+        <v>52438</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="G34" s="7">
-        <v>1306.458212</v>
+        <v>1921.785116</v>
       </c>
       <c r="H34" s="11">
-        <v>1306</v>
+        <v>1922</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
@@ -1689,13 +1600,13 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="9">
-        <v>1817.28</v>
+        <v>60219</v>
       </c>
       <c r="C35" s="9">
-        <v>1817</v>
+        <v>60219</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1712,21 +1623,21 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" s="9">
-        <v>50683</v>
+        <v>30350</v>
       </c>
       <c r="C36" s="9">
-        <v>50683</v>
+        <v>30350</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="G36" s="7">
-        <v>1724.73188</v>
+        <v>591.94788000000005</v>
       </c>
       <c r="H36" s="11">
-        <v>1725</v>
+        <v>592</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -1737,21 +1648,21 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="9">
-        <v>21848</v>
+        <v>6126</v>
       </c>
       <c r="C37" s="9">
-        <v>21848</v>
+        <v>6126</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="G37" s="7">
-        <v>767.7</v>
+        <v>204.54939999999999</v>
       </c>
       <c r="H37" s="11">
-        <v>768</v>
+        <v>205</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -1762,20 +1673,22 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="9">
-        <v>1817.28</v>
+        <v>12614</v>
       </c>
       <c r="C38" s="9">
-        <v>1817</v>
+        <v>12614</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="G38" s="7">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11"/>
+        <v>421.12268799999998</v>
+      </c>
+      <c r="H38" s="11">
+        <v>421</v>
+      </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="M38" s="13"/>
@@ -1785,21 +1698,21 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="9">
-        <v>99519</v>
+        <v>16277</v>
       </c>
       <c r="C39" s="9">
-        <v>99519</v>
+        <v>16277</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="G39" s="7">
-        <v>3409.7822000000001</v>
+        <v>331.574748</v>
       </c>
       <c r="H39" s="11">
-        <v>3410</v>
+        <v>332</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
@@ -1810,22 +1723,20 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="9">
-        <v>16989</v>
+        <v>6422</v>
       </c>
       <c r="C40" s="9">
-        <v>16989</v>
+        <v>6422</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="G40" s="7">
-        <v>616.02636399999994</v>
-      </c>
-      <c r="H40" s="11">
-        <v>616</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H40" s="11"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="M40" s="13"/>
@@ -1835,21 +1746,21 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="9">
-        <v>36997</v>
+        <v>96536</v>
       </c>
       <c r="C41" s="9">
-        <v>36997</v>
+        <v>96536</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="G41" s="7">
-        <v>1341.4789800000001</v>
+        <v>3025.5909999999999</v>
       </c>
       <c r="H41" s="11">
-        <v>1341</v>
+        <v>3026</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
@@ -1860,20 +1771,22 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="9">
-        <v>45035</v>
+        <v>39132</v>
       </c>
       <c r="C42" s="9">
-        <v>45035</v>
+        <v>39132</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="G42" s="7">
-        <v>0</v>
-      </c>
-      <c r="H42" s="11"/>
+        <v>1306.458212</v>
+      </c>
+      <c r="H42" s="11">
+        <v>1306</v>
+      </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="M42" s="13"/>
@@ -1883,22 +1796,20 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="9">
-        <v>70327</v>
+        <v>1817.28</v>
       </c>
       <c r="C43" s="9">
-        <v>70327</v>
+        <v>1817</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="G43" s="7">
-        <v>2525.9036000000001</v>
-      </c>
-      <c r="H43" s="11">
-        <v>2526</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H43" s="11"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="M43" s="13"/>
@@ -1908,21 +1819,21 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="9">
-        <v>62439</v>
+        <v>50683</v>
       </c>
       <c r="C44" s="9">
-        <v>62439</v>
+        <v>50683</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="G44" s="7">
-        <v>2298.16966</v>
+        <v>1724.73188</v>
       </c>
       <c r="H44" s="11">
-        <v>2298</v>
+        <v>1725</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
@@ -1933,21 +1844,21 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" s="9">
-        <v>26886</v>
+        <v>21848</v>
       </c>
       <c r="C45" s="9">
-        <v>26886</v>
+        <v>21848</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="G45" s="7">
-        <v>989.60283200000003</v>
+        <v>767.7</v>
       </c>
       <c r="H45" s="11">
-        <v>990</v>
+        <v>768</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -1958,13 +1869,13 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="9">
-        <v>30254</v>
+        <v>1817.28</v>
       </c>
       <c r="C46" s="9">
-        <v>30254</v>
+        <v>1817</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -1981,21 +1892,21 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="9">
-        <v>73579</v>
+        <v>99519</v>
       </c>
       <c r="C47" s="9">
-        <v>73579</v>
+        <v>99519</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="G47" s="7">
-        <v>2305.3519200000001</v>
+        <v>3409.7822000000001</v>
       </c>
       <c r="H47" s="11">
-        <v>2305</v>
+        <v>3410</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -2006,21 +1917,21 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="9">
-        <v>32640</v>
+        <v>16989</v>
       </c>
       <c r="C48" s="9">
-        <v>32640</v>
+        <v>16989</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="G48" s="7">
-        <v>1014.28524</v>
+        <v>616.02636399999994</v>
       </c>
       <c r="H48" s="11">
-        <v>1014</v>
+        <v>616</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
@@ -2031,20 +1942,22 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="9">
-        <v>14816</v>
+        <v>36997</v>
       </c>
       <c r="C49" s="9">
-        <v>14816</v>
+        <v>36997</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="G49" s="7">
-        <v>0</v>
-      </c>
-      <c r="H49" s="11"/>
+        <v>1341.4789800000001</v>
+      </c>
+      <c r="H49" s="11">
+        <v>1341</v>
+      </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="M49" s="13"/>
@@ -2054,22 +1967,20 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="9">
-        <v>89230.997700000007</v>
+        <v>45035</v>
       </c>
       <c r="C50" s="9">
-        <v>89231</v>
+        <v>45035</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="G50" s="7">
-        <v>2365.1984000000002</v>
-      </c>
-      <c r="H50" s="11">
-        <v>2365</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H50" s="11"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="M50" s="13"/>
@@ -2079,21 +1990,21 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51" s="9">
-        <v>58047</v>
+        <v>70327</v>
       </c>
       <c r="C51" s="9">
-        <v>58047</v>
+        <v>70327</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="G51" s="7">
-        <v>1830.4527</v>
+        <v>2525.9036000000001</v>
       </c>
       <c r="H51" s="11">
-        <v>1830</v>
+        <v>2526</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -2104,21 +2015,21 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="9">
-        <v>122667</v>
+        <v>62439</v>
       </c>
       <c r="C52" s="9">
-        <v>122667</v>
+        <v>62439</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="G52" s="7">
-        <v>3683.4245999999998</v>
+        <v>2298.16966</v>
       </c>
       <c r="H52" s="11">
-        <v>3683</v>
+        <v>2298</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
@@ -2129,21 +2040,21 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="9">
-        <v>48008</v>
+        <v>26886</v>
       </c>
       <c r="C53" s="9">
-        <v>48008</v>
+        <v>26886</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="G53" s="7">
-        <v>1513.9043999999999</v>
+        <v>989.60283200000003</v>
       </c>
       <c r="H53" s="11">
-        <v>1514</v>
+        <v>990</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -2154,13 +2065,13 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" s="9">
-        <v>47755</v>
+        <v>30254</v>
       </c>
       <c r="C54" s="9">
-        <v>47755</v>
+        <v>30254</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -2176,16 +2087,23 @@
       <c r="P54" s="1"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
       <c r="B55" s="9">
-        <v>1942029.96199376</v>
-      </c>
-      <c r="C55" s="9"/>
+        <v>73579</v>
+      </c>
+      <c r="C55" s="9">
+        <v>73579</v>
+      </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="G55" s="7">
-        <v>57171.01823675519</v>
-      </c>
-      <c r="H55" s="11"/>
+        <v>2305.3519200000001</v>
+      </c>
+      <c r="H55" s="11">
+        <v>2305</v>
+      </c>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="M55" s="13"/>
@@ -2194,12 +2112,23 @@
       <c r="P55" s="1"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="9">
+        <v>32640</v>
+      </c>
+      <c r="C56" s="9">
+        <v>32640</v>
+      </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="11"/>
+      <c r="G56" s="7">
+        <v>1014.28524</v>
+      </c>
+      <c r="H56" s="11">
+        <v>1014</v>
+      </c>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="M56" s="13"/>
@@ -2208,11 +2137,20 @@
       <c r="P56" s="1"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="9">
+        <v>14816</v>
+      </c>
+      <c r="C57" s="9">
+        <v>14816</v>
+      </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="G57" s="7"/>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
       <c r="H57" s="11"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -2222,12 +2160,23 @@
       <c r="P57" s="1"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="9">
+        <v>89230.997700000007</v>
+      </c>
+      <c r="C58" s="9">
+        <v>89231</v>
+      </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="11"/>
+      <c r="G58" s="7">
+        <v>2365.1984000000002</v>
+      </c>
+      <c r="H58" s="11">
+        <v>2365</v>
+      </c>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="M58" s="13"/>
@@ -2236,12 +2185,23 @@
       <c r="P58" s="1"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="9">
+        <v>58047</v>
+      </c>
+      <c r="C59" s="9">
+        <v>58047</v>
+      </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="11"/>
+      <c r="G59" s="7">
+        <v>1830.4527</v>
+      </c>
+      <c r="H59" s="11">
+        <v>1830</v>
+      </c>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="M59" s="13"/>
@@ -2250,12 +2210,23 @@
       <c r="P59" s="1"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="9">
+        <v>122667</v>
+      </c>
+      <c r="C60" s="9">
+        <v>122667</v>
+      </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="11"/>
+      <c r="G60" s="7">
+        <v>3683.4245999999998</v>
+      </c>
+      <c r="H60" s="11">
+        <v>3683</v>
+      </c>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="M60" s="13"/>
@@ -2264,12 +2235,23 @@
       <c r="P60" s="1"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="9">
+        <v>48008</v>
+      </c>
+      <c r="C61" s="9">
+        <v>48008</v>
+      </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="11"/>
+      <c r="G61" s="7">
+        <v>1513.9043999999999</v>
+      </c>
+      <c r="H61" s="11">
+        <v>1514</v>
+      </c>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="M61" s="13"/>
@@ -2278,11 +2260,20 @@
       <c r="P61" s="1"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="9">
+        <v>47755</v>
+      </c>
+      <c r="C62" s="9">
+        <v>47755</v>
+      </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
-      <c r="G62" s="7"/>
+      <c r="G62" s="7">
+        <v>0</v>
+      </c>
       <c r="H62" s="11"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -2292,11 +2283,15 @@
       <c r="P62" s="1"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B63" s="9"/>
+      <c r="B63" s="9">
+        <v>1942029.96199376</v>
+      </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
-      <c r="G63" s="7"/>
+      <c r="G63" s="7">
+        <v>57171.01823675519</v>
+      </c>
       <c r="H63" s="11"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -5035,25 +5030,138 @@
       <c r="O258" s="1"/>
       <c r="P258" s="1"/>
     </row>
+    <row r="259" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B259" s="9"/>
+      <c r="C259" s="9"/>
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="G259" s="7"/>
+      <c r="H259" s="11"/>
+      <c r="I259" s="7"/>
+      <c r="J259" s="7"/>
+      <c r="M259" s="13"/>
+      <c r="N259" s="1"/>
+      <c r="O259" s="1"/>
+      <c r="P259" s="1"/>
+    </row>
+    <row r="260" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B260" s="9"/>
+      <c r="C260" s="9"/>
+      <c r="D260" s="9"/>
+      <c r="E260" s="9"/>
+      <c r="G260" s="7"/>
+      <c r="H260" s="11"/>
+      <c r="I260" s="7"/>
+      <c r="J260" s="7"/>
+      <c r="M260" s="13"/>
+      <c r="N260" s="1"/>
+      <c r="O260" s="1"/>
+      <c r="P260" s="1"/>
+    </row>
+    <row r="261" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B261" s="9"/>
+      <c r="C261" s="9"/>
+      <c r="D261" s="9"/>
+      <c r="E261" s="9"/>
+      <c r="G261" s="7"/>
+      <c r="H261" s="11"/>
+      <c r="I261" s="7"/>
+      <c r="J261" s="7"/>
+      <c r="M261" s="13"/>
+      <c r="N261" s="1"/>
+      <c r="O261" s="1"/>
+      <c r="P261" s="1"/>
+    </row>
+    <row r="262" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B262" s="9"/>
+      <c r="C262" s="9"/>
+      <c r="D262" s="9"/>
+      <c r="E262" s="9"/>
+      <c r="G262" s="7"/>
+      <c r="H262" s="11"/>
+      <c r="I262" s="7"/>
+      <c r="J262" s="7"/>
+      <c r="M262" s="13"/>
+      <c r="N262" s="1"/>
+      <c r="O262" s="1"/>
+      <c r="P262" s="1"/>
+    </row>
+    <row r="263" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="G263" s="7"/>
+      <c r="H263" s="11"/>
+      <c r="I263" s="7"/>
+      <c r="J263" s="7"/>
+      <c r="M263" s="13"/>
+      <c r="N263" s="1"/>
+      <c r="O263" s="1"/>
+      <c r="P263" s="1"/>
+    </row>
+    <row r="264" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B264" s="9"/>
+      <c r="C264" s="9"/>
+      <c r="D264" s="9"/>
+      <c r="E264" s="9"/>
+      <c r="G264" s="7"/>
+      <c r="H264" s="11"/>
+      <c r="I264" s="7"/>
+      <c r="J264" s="7"/>
+      <c r="M264" s="13"/>
+      <c r="N264" s="1"/>
+      <c r="O264" s="1"/>
+      <c r="P264" s="1"/>
+    </row>
+    <row r="265" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B265" s="9"/>
+      <c r="C265" s="9"/>
+      <c r="D265" s="9"/>
+      <c r="E265" s="9"/>
+      <c r="G265" s="7"/>
+      <c r="H265" s="11"/>
+      <c r="I265" s="7"/>
+      <c r="J265" s="7"/>
+      <c r="M265" s="13"/>
+      <c r="N265" s="1"/>
+      <c r="O265" s="1"/>
+      <c r="P265" s="1"/>
+    </row>
+    <row r="266" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B266" s="9"/>
+      <c r="C266" s="9"/>
+      <c r="D266" s="9"/>
+      <c r="E266" s="9"/>
+      <c r="G266" s="7"/>
+      <c r="H266" s="11"/>
+      <c r="I266" s="7"/>
+      <c r="J266" s="7"/>
+      <c r="M266" s="13"/>
+      <c r="N266" s="1"/>
+      <c r="O266" s="1"/>
+      <c r="P266" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G4:H4"/>
+  <mergeCells count="14">
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
-  <conditionalFormatting sqref="H7:H258 C9:C258">
+  <conditionalFormatting sqref="C15:C266 H15:H266">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(NOT(ISBLANK(C7)), ROUND(C7, 0) &lt;&gt; ROUND(B7, 0))</formula>
+      <formula>AND(NOT(ISBLANK(C15)), ROUND(C15, 0) &lt;&gt; ROUND(B15, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
freeze headings/titles in Comparator.xlsx
</commit_message>
<xml_diff>
--- a/Comparator.xlsx
+++ b/Comparator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coder\Desktop\WordExcelComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B1985D-564C-46CD-A912-C6B2BBB82E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE1FEC-87CE-40E4-86D1-9EE27863C055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5063" yWindow="90" windowWidth="23684" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="225" windowWidth="23175" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparator" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -600,21 +600,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1065,7 +1065,10 @@
   <dimension ref="A2:CV266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP26" sqref="AP26"/>
+      <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1157,7 +1160,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:100" x14ac:dyDescent="0.45">
@@ -1414,105 +1417,105 @@
       </c>
     </row>
     <row r="10" spans="1:100" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="41"/>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="43" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="41"/>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="43" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="41"/>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="43" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="41"/>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="43" t="s">
         <v>13</v>
       </c>
       <c r="M10" s="40"/>
       <c r="N10" s="41"/>
-      <c r="Q10" s="39" t="s">
+      <c r="Q10" s="43" t="s">
         <v>14</v>
       </c>
       <c r="R10" s="40"/>
       <c r="S10" s="41"/>
-      <c r="V10" s="39" t="s">
+      <c r="V10" s="43" t="s">
         <v>15</v>
       </c>
       <c r="W10" s="40"/>
       <c r="X10" s="41"/>
-      <c r="AA10" s="39" t="s">
+      <c r="AA10" s="43" t="s">
         <v>16</v>
       </c>
       <c r="AB10" s="40"/>
       <c r="AC10" s="41"/>
-      <c r="AF10" s="39" t="s">
+      <c r="AF10" s="43" t="s">
         <v>17</v>
       </c>
       <c r="AG10" s="40"/>
       <c r="AH10" s="41"/>
-      <c r="AK10" s="39" t="s">
+      <c r="AK10" s="43" t="s">
         <v>18</v>
       </c>
       <c r="AL10" s="40"/>
       <c r="AM10" s="41"/>
-      <c r="AP10" s="39" t="s">
+      <c r="AP10" s="43" t="s">
         <v>19</v>
       </c>
       <c r="AQ10" s="40"/>
       <c r="AR10" s="41"/>
-      <c r="AU10" s="39" t="s">
+      <c r="AU10" s="43" t="s">
         <v>20</v>
       </c>
       <c r="AV10" s="40"/>
       <c r="AW10" s="41"/>
-      <c r="AZ10" s="39" t="s">
+      <c r="AZ10" s="43" t="s">
         <v>21</v>
       </c>
       <c r="BA10" s="40"/>
       <c r="BB10" s="41"/>
-      <c r="BE10" s="39" t="s">
+      <c r="BE10" s="43" t="s">
         <v>22</v>
       </c>
       <c r="BF10" s="40"/>
       <c r="BG10" s="41"/>
-      <c r="BJ10" s="39" t="s">
+      <c r="BJ10" s="43" t="s">
         <v>23</v>
       </c>
       <c r="BK10" s="40"/>
       <c r="BL10" s="41"/>
-      <c r="BO10" s="39" t="s">
+      <c r="BO10" s="43" t="s">
         <v>24</v>
       </c>
       <c r="BP10" s="40"/>
       <c r="BQ10" s="41"/>
-      <c r="BT10" s="39" t="s">
+      <c r="BT10" s="43" t="s">
         <v>25</v>
       </c>
       <c r="BU10" s="40"/>
       <c r="BV10" s="41"/>
-      <c r="BY10" s="39" t="s">
+      <c r="BY10" s="43" t="s">
         <v>26</v>
       </c>
       <c r="BZ10" s="40"/>
       <c r="CA10" s="41"/>
-      <c r="CD10" s="39" t="s">
+      <c r="CD10" s="43" t="s">
         <v>27</v>
       </c>
       <c r="CE10" s="40"/>
       <c r="CF10" s="41"/>
-      <c r="CI10" s="39" t="s">
+      <c r="CI10" s="43" t="s">
         <v>28</v>
       </c>
       <c r="CJ10" s="40"/>
       <c r="CK10" s="41"/>
-      <c r="CN10" s="39" t="s">
+      <c r="CN10" s="43" t="s">
         <v>29</v>
       </c>
       <c r="CO10" s="40"/>
@@ -1524,7 +1527,7 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="41"/>
-      <c r="D11" s="49"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="40"/>
       <c r="F11" s="41"/>
       <c r="G11" s="42"/>
@@ -1639,19 +1642,19 @@
       <c r="A12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="44"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="45"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="47"/>
       <c r="M12" s="45"/>
-      <c r="N12" s="47"/>
+      <c r="N12" s="46"/>
       <c r="O12" t="s">
         <v>33</v>
       </c>
@@ -6327,9 +6330,7 @@
       <c r="CV62" s="1"/>
     </row>
     <row r="63" spans="2:100" x14ac:dyDescent="0.45">
-      <c r="B63" s="8">
-        <v>1942029.96199376</v>
-      </c>
+      <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
@@ -24080,22 +24081,38 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="BO11:BQ11"/>
-    <mergeCell ref="BT12:BV12"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AF10:AH10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="BT10:BV10"/>
-    <mergeCell ref="CI11:CK11"/>
-    <mergeCell ref="CD12:CF12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="BJ11:BL11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="AF12:AH12"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="BY12:CA12"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="CD10:CF10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="BY11:CA11"/>
+    <mergeCell ref="CN10:CP10"/>
+    <mergeCell ref="BY10:CA10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="AZ10:BB10"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="CD11:CF11"/>
+    <mergeCell ref="BT11:BV11"/>
+    <mergeCell ref="BJ10:BL10"/>
+    <mergeCell ref="AU10:AW10"/>
+    <mergeCell ref="CI10:CK10"/>
+    <mergeCell ref="CN11:CP11"/>
+    <mergeCell ref="CN12:CP12"/>
+    <mergeCell ref="AU11:AW11"/>
+    <mergeCell ref="AF11:AH11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="BE11:BG11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="BJ12:BL12"/>
+    <mergeCell ref="AZ12:BB12"/>
+    <mergeCell ref="CI12:CK12"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="Q11:S11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="BO12:BQ12"/>
     <mergeCell ref="BE12:BG12"/>
@@ -24112,38 +24129,22 @@
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="AK12:AM12"/>
     <mergeCell ref="V10:X10"/>
-    <mergeCell ref="CN12:CP12"/>
-    <mergeCell ref="AU11:AW11"/>
-    <mergeCell ref="AF11:AH11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="BE11:BG11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="BJ12:BL12"/>
-    <mergeCell ref="AZ12:BB12"/>
-    <mergeCell ref="CI12:CK12"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="CD10:CF10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BY11:CA11"/>
-    <mergeCell ref="CN10:CP10"/>
-    <mergeCell ref="BY10:CA10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="AZ10:BB10"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="CD11:CF11"/>
-    <mergeCell ref="BT11:BV11"/>
-    <mergeCell ref="BJ10:BL10"/>
-    <mergeCell ref="AU10:AW10"/>
-    <mergeCell ref="CI10:CK10"/>
-    <mergeCell ref="CN11:CP11"/>
+    <mergeCell ref="CI11:CK11"/>
+    <mergeCell ref="CD12:CF12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="BJ11:BL11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="BY12:CA12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="BO11:BQ11"/>
+    <mergeCell ref="BT12:BV12"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AF10:AH10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="BT10:BV10"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:C266 H15:H266">
     <cfRule type="expression" dxfId="17" priority="18">

</xml_diff>

<commit_message>
debug previous: refactor for 2D alias array with 5 aliases per data point, 5 ouput columns per data point in Comparator.xlsx
</commit_message>
<xml_diff>
--- a/Comparator.xlsx
+++ b/Comparator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coder\Desktop\WordExcelComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32382BA-7EFF-4CA2-B522-6C7396751FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67B4B16-31C7-4526-B925-1A0A8AB6BB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="308" yWindow="300" windowWidth="26092" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1267" yWindow="255" windowWidth="22305" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparator" sheetId="1" r:id="rId1"/>
@@ -30,30 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
   <si>
     <t>Project Name</t>
   </si>
@@ -76,6 +54,9 @@
     <t>Total Discrepancies Found</t>
   </si>
   <si>
+    <t>Error per alias/data point</t>
+  </si>
+  <si>
     <t>Discrepancies</t>
   </si>
   <si>
@@ -83,6 +64,9 @@
   </si>
   <si>
     <t>Total energy savings (MBTU/yr) from Y258</t>
+  </si>
+  <si>
+    <t>Annual Estimated Energy Savings (MMBtu)</t>
   </si>
   <si>
     <t>ECM cost savings from column AE</t>
@@ -142,6 +126,30 @@
     <t>Simple Payback Period column AG</t>
   </si>
   <si>
+    <t xml:space="preserve"> Total Utility ($/yr) Cost Savings Year 1 </t>
+  </si>
+  <si>
+    <t>Total Energy (mmBTU) Savings Year 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project ($) Cost </t>
+  </si>
+  <si>
+    <t>Electricity Consumption  (kWh/yr) Savings Year 1</t>
+  </si>
+  <si>
+    <t>Electricity Demand  (kW/mo) Savings Year 1</t>
+  </si>
+  <si>
+    <t>Nat Gas Consumption  (MMBTU/yr) Savings Year 1</t>
+  </si>
+  <si>
+    <t>Water Sewer Consumption (kGal) Savings Year 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Pay back </t>
+  </si>
+  <si>
     <t>ECMs by Building</t>
   </si>
   <si>
@@ -155,6 +163,21 @@
   </si>
   <si>
     <t>ePB Sch 4 Savings</t>
+  </si>
+  <si>
+    <t>Alias 1</t>
+  </si>
+  <si>
+    <t>Alias 2</t>
+  </si>
+  <si>
+    <t>Alias 3</t>
+  </si>
+  <si>
+    <t>Alias 4</t>
+  </si>
+  <si>
+    <t>Alias 5</t>
   </si>
   <si>
     <t>MBTU/yr Savings</t>
@@ -172,7 +195,7 @@
     <t>Baseline kW</t>
   </si>
   <si>
-    <t>Baseline Gas Mbtu</t>
+    <t>Baseline Gas MBTU</t>
   </si>
   <si>
     <t>Baseline Kgal</t>
@@ -228,24 +251,6 @@
   <si>
     <t>Total</t>
   </si>
-  <si>
-    <t>Alias 1</t>
-  </si>
-  <si>
-    <t>Alias 2</t>
-  </si>
-  <si>
-    <t>Alias 3</t>
-  </si>
-  <si>
-    <t>Alias 4</t>
-  </si>
-  <si>
-    <t>Alias 5</t>
-  </si>
-  <si>
-    <t>Error per alias/data point</t>
-  </si>
 </sst>
 </file>
 
@@ -255,7 +260,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +286,21 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4C4E52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF4C4E52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -533,21 +553,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -558,7 +589,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -619,47 +650,45 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +699,14 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1113,7 +1149,7 @@
       <pane xSplit="1" ySplit="15" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1132,7 +1168,7 @@
     <col min="13" max="13" width="18.59765625" customWidth="1"/>
     <col min="14" max="14" width="20.796875" customWidth="1"/>
     <col min="15" max="15" width="18.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="16" max="16" width="15.1328125" customWidth="1"/>
     <col min="17" max="17" width="16.3984375" customWidth="1"/>
     <col min="18" max="19" width="14.9296875" customWidth="1"/>
     <col min="20" max="20" width="16.59765625" customWidth="1"/>
@@ -1147,11 +1183,11 @@
     <col min="32" max="32" width="16.3984375" customWidth="1"/>
     <col min="33" max="34" width="14.9296875" customWidth="1"/>
     <col min="35" max="35" width="13.9296875" customWidth="1"/>
-    <col min="36" max="36" width="12.19921875" customWidth="1"/>
+    <col min="36" max="36" width="16.1328125" customWidth="1"/>
     <col min="37" max="37" width="16.3984375" customWidth="1"/>
     <col min="38" max="41" width="14.9296875" customWidth="1"/>
     <col min="42" max="42" width="18.06640625" customWidth="1"/>
-    <col min="43" max="43" width="10.3984375" customWidth="1"/>
+    <col min="43" max="43" width="12.06640625" customWidth="1"/>
     <col min="44" max="44" width="16.3984375" customWidth="1"/>
     <col min="45" max="48" width="14.9296875" customWidth="1"/>
     <col min="49" max="49" width="16.6640625" customWidth="1"/>
@@ -1220,8 +1256,8 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -1246,9 +1282,6 @@
         <v>4</v>
       </c>
       <c r="B6" s="18"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -1267,757 +1300,667 @@
     </row>
     <row r="9" spans="1:138" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="C9" s="15" cm="1">
+      <c r="C9" s="15">
         <f t="array" ref="C9">SUM(IF(ROUND($B16:$B267,0)&lt;&gt;ROUND(C16:C267,0), 1, 0)) + COUNTBLANK($B16:$B267) + COUNTIF($B16:$B267, 0) - COUNTBLANK(C16:C267) - COUNTIF(C16:C267, 0)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="15" cm="1">
+      <c r="D9" s="15">
         <f t="array" ref="D9">SUM(IF(ROUND($B16:$B267,0)&lt;&gt;ROUND(D16:D267,0), 1, 0)) + COUNTBLANK($B16:$B267) + COUNTIF($B16:$B267, 0) - COUNTBLANK(D16:D267) - COUNTIF(D16:D267, 0)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="15" cm="1">
+      <c r="E9" s="15">
         <f t="array" ref="E9">SUM(IF(ROUND($B16:$B267,0)&lt;&gt;ROUND(E16:E267,0), 1, 0)) + COUNTBLANK($B16:$B267) + COUNTIF($B16:$B267, 0) - COUNTBLANK(E16:E267) - COUNTIF(E16:E267, 0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="15" cm="1">
+      <c r="F9" s="15">
         <f t="array" ref="F9">SUM(IF(ROUND($B16:$B267,0)&lt;&gt;ROUND(F16:F267,0), 1, 0)) + COUNTBLANK($B16:$B267) + COUNTIF($B16:$B267, 0) - COUNTBLANK(F16:F267) - COUNTIF(F16:F267, 0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="15" cm="1">
+      <c r="G9" s="15">
         <f t="array" ref="G9">SUM(IF(ROUND($B16:$B267,0)&lt;&gt;ROUND(G16:G267,0), 1, 0)) + COUNTBLANK($B16:$B267) + COUNTIF($B16:$B267, 0) - COUNTBLANK(G16:G267) - COUNTIF(G16:G267, 0)</f>
         <v>0</v>
       </c>
       <c r="I9" s="15"/>
-      <c r="J9" s="15" cm="1">
+      <c r="J9" s="15">
         <f t="array" ref="J9">SUM(IF(ROUND($I16:$I267,0)&lt;&gt;ROUND(J16:J267,0), 1, 0)) + COUNTBLANK($I16:$I267) + COUNTIF($I16:$I267, 0) - COUNTBLANK(J16:J267) - COUNTIF(J16:J267, 0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="15" cm="1">
+      <c r="K9" s="15">
         <f t="array" ref="K9">SUM(IF(ROUND($I16:$I267,0)&lt;&gt;ROUND(K16:K267,0), 1, 0)) + COUNTBLANK($I16:$I267) + COUNTIF($I16:$I267, 0) - COUNTBLANK(K16:K267) - COUNTIF(K16:K267, 0)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="15" cm="1">
+      <c r="L9" s="15">
         <f t="array" ref="L9">SUM(IF(ROUND($I16:$I267,0)&lt;&gt;ROUND(L16:L267,0), 1, 0)) + COUNTBLANK($I16:$I267) + COUNTIF($I16:$I267, 0) - COUNTBLANK(L16:L267) - COUNTIF(L16:L267, 0)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="15" cm="1">
+      <c r="M9" s="15">
         <f t="array" ref="M9">SUM(IF(ROUND($I16:$I267,0)&lt;&gt;ROUND(M16:M267,0), 1, 0)) + COUNTBLANK($I16:$I267) + COUNTIF($I16:$I267, 0) - COUNTBLANK(M16:M267) - COUNTIF(M16:M267, 0)</f>
         <v>0</v>
       </c>
-      <c r="N9" s="15" cm="1">
+      <c r="N9" s="15">
         <f t="array" ref="N9">SUM(IF(ROUND($I16:$I267,0)&lt;&gt;ROUND(N16:N267,0), 1, 0)) + COUNTBLANK($I16:$I267) + COUNTIF($I16:$I267, 0) - COUNTBLANK(N16:N267) - COUNTIF(N16:N267, 0)</f>
         <v>0</v>
       </c>
-      <c r="O9" s="15"/>
-      <c r="Q9" s="17" cm="1">
+      <c r="Q9" s="17">
         <f t="array" ref="Q9">SUM(IF(ROUND($P16:$P267,0)&lt;&gt;ROUND(Q16:Q267,0), 1, 0)) + COUNTBLANK($P16:$P267) + COUNTIF($P16:$P267, 0) - COUNTBLANK(Q16:Q267) - COUNTIF(Q16:Q267, 0)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="17" cm="1">
+      <c r="R9" s="17">
         <f t="array" ref="R9">SUM(IF(ROUND($P16:$P267,0)&lt;&gt;ROUND(R16:R267,0), 1, 0)) + COUNTBLANK($P16:$P267) + COUNTIF($P16:$P267, 0) - COUNTBLANK(R16:R267) - COUNTIF(R16:R267, 0)</f>
         <v>0</v>
       </c>
-      <c r="S9" s="17" cm="1">
+      <c r="S9" s="17">
         <f t="array" ref="S9">SUM(IF(ROUND($P16:$P267,0)&lt;&gt;ROUND(S16:S267,0), 1, 0)) + COUNTBLANK($P16:$P267) + COUNTIF($P16:$P267, 0) - COUNTBLANK(S16:S267) - COUNTIF(S16:S267, 0)</f>
         <v>0</v>
       </c>
-      <c r="T9" s="17" cm="1">
+      <c r="T9" s="17">
         <f t="array" ref="T9">SUM(IF(ROUND($P16:$P267,0)&lt;&gt;ROUND(T16:T267,0), 1, 0)) + COUNTBLANK($P16:$P267) + COUNTIF($P16:$P267, 0) - COUNTBLANK(T16:T267) - COUNTIF(T16:T267, 0)</f>
         <v>0</v>
       </c>
-      <c r="U9" s="17" cm="1">
+      <c r="U9" s="17">
         <f t="array" ref="U9">SUM(IF(ROUND($P16:$P267,0)&lt;&gt;ROUND(U16:U267,0), 1, 0)) + COUNTBLANK($P16:$P267) + COUNTIF($P16:$P267, 0) - COUNTBLANK(U16:U267) - COUNTIF(U16:U267, 0)</f>
         <v>0</v>
       </c>
-      <c r="X9" s="17" cm="1">
+      <c r="X9" s="17">
         <f t="array" ref="X9">SUM(IF(ROUND($W16:$W267,0)&lt;&gt;ROUND(X16:X267,0), 1, 0)) + COUNTBLANK($W16:$W267) + COUNTIF($W16:$W267, 0) - COUNTBLANK(X16:X267) - COUNTIF(X16:X267, 0)</f>
         <v>0</v>
       </c>
-      <c r="Y9" s="17" cm="1">
+      <c r="Y9" s="17">
         <f t="array" ref="Y9">SUM(IF(ROUND($W16:$W267,0)&lt;&gt;ROUND(Y16:Y267,0), 1, 0)) + COUNTBLANK($W16:$W267) + COUNTIF($W16:$W267, 0) - COUNTBLANK(Y16:Y267) - COUNTIF(Y16:Y267, 0)</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="17" cm="1">
+      <c r="Z9" s="17">
         <f t="array" ref="Z9">SUM(IF(ROUND($W16:$W267,0)&lt;&gt;ROUND(Z16:Z267,0), 1, 0)) + COUNTBLANK($W16:$W267) + COUNTIF($W16:$W267, 0) - COUNTBLANK(Z16:Z267) - COUNTIF(Z16:Z267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AA9" s="17" cm="1">
+      <c r="AA9" s="17">
         <f t="array" ref="AA9">SUM(IF(ROUND($W16:$W267,0)&lt;&gt;ROUND(AA16:AA267,0), 1, 0)) + COUNTBLANK($W16:$W267) + COUNTIF($W16:$W267, 0) - COUNTBLANK(AA16:AA267) - COUNTIF(AA16:AA267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AB9" s="17" cm="1">
+      <c r="AB9" s="17">
         <f t="array" ref="AB9">SUM(IF(ROUND($W16:$W267,0)&lt;&gt;ROUND(AB16:AB267,0), 1, 0)) + COUNTBLANK($W16:$W267) + COUNTIF($W16:$W267, 0) - COUNTBLANK(AB16:AB267) - COUNTIF(AB16:AB267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AE9" s="17" cm="1">
+      <c r="AE9" s="17">
         <f t="array" ref="AE9">SUM(IF(ROUND(AD16:AD267,0)&lt;&gt;ROUND(AE16:AE267,0), 1, 0)) + COUNTBLANK(AD16:AD267) + COUNTIF(AD16:AD267, 0) - COUNTBLANK(AE16:AE267) - COUNTIF(AE16:AE267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AF9" s="17" cm="1">
+      <c r="AF9" s="17">
         <f t="array" ref="AF9">SUM(IF(ROUND(AD16:AD267,0)&lt;&gt;ROUND(AF16:AF267,0), 1, 0)) + COUNTBLANK(AD16:AD267) + COUNTIF(AD16:AD267, 0) - COUNTBLANK(AF16:AF267) - COUNTIF(AF16:AF267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AG9" s="17" cm="1">
+      <c r="AG9" s="17">
         <f t="array" ref="AG9">SUM(IF(ROUND(AD16:AD267,0)&lt;&gt;ROUND(AG16:AG267,0), 1, 0)) + COUNTBLANK(AD16:AD267) + COUNTIF(AD16:AD267, 0) - COUNTBLANK(AG16:AG267) - COUNTIF(AG16:AG267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AH9" s="17" cm="1">
+      <c r="AH9" s="17">
         <f t="array" ref="AH9">SUM(IF(ROUND(AD16:AD267,0)&lt;&gt;ROUND(AH16:AH267,0), 1, 0)) + COUNTBLANK(AD16:AD267) + COUNTIF(AD16:AD267, 0) - COUNTBLANK(AH16:AH267) - COUNTIF(AH16:AH267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AI9" s="17" cm="1">
+      <c r="AI9" s="17">
         <f t="array" ref="AI9">SUM(IF(ROUND(AD16:AD267,0)&lt;&gt;ROUND(AI16:AI267,0), 1, 0)) + COUNTBLANK(AD16:AD267) + COUNTIF(AD16:AD267, 0) - COUNTBLANK(AI16:AI267) - COUNTIF(AI16:AI267, 0)</f>
         <v>0</v>
       </c>
       <c r="AK9" s="17"/>
-      <c r="AL9" s="17" cm="1">
+      <c r="AL9" s="17">
         <f t="array" ref="AL9">SUM(IF(ROUND(AK16:AK267,0)&lt;&gt;ROUND(AL16:AL267,0), 1, 0)) + COUNTBLANK(AK16:AK267) + COUNTIF(AK16:AK267, 0) - COUNTBLANK(AL16:AL267) - COUNTIF(AL16:AL267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AM9" s="17" cm="1">
+      <c r="AM9" s="17">
         <f t="array" ref="AM9">SUM(IF(ROUND(AK16:AK267,0)&lt;&gt;ROUND(AM16:AM267,0), 1, 0)) + COUNTBLANK(AK16:AK267) + COUNTIF(AK16:AK267, 0) - COUNTBLANK(AM16:AM267) - COUNTIF(AM16:AM267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AN9" s="17" cm="1">
+      <c r="AN9" s="17">
         <f t="array" ref="AN9">SUM(IF(ROUND(AK16:AK267,0)&lt;&gt;ROUND(AN16:AN267,0), 1, 0)) + COUNTBLANK(AK16:AK267) + COUNTIF(AK16:AK267, 0) - COUNTBLANK(AN16:AN267) - COUNTIF(AN16:AN267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AO9" s="17" cm="1">
+      <c r="AO9" s="17">
         <f t="array" ref="AO9">SUM(IF(ROUND(AK16:AK267,0)&lt;&gt;ROUND(AO16:AO267,0), 1, 0)) + COUNTBLANK(AK16:AK267) + COUNTIF(AK16:AK267, 0) - COUNTBLANK(AO16:AO267) - COUNTIF(AO16:AO267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AP9" s="17" cm="1">
+      <c r="AP9" s="17">
         <f t="array" ref="AP9">SUM(IF(ROUND(AK16:AK267,0)&lt;&gt;ROUND(AP16:AP267,0), 1, 0)) + COUNTBLANK(AK16:AK267) + COUNTIF(AK16:AK267, 0) - COUNTBLANK(AP16:AP267) - COUNTIF(AP16:AP267, 0)</f>
         <v>0</v>
       </c>
       <c r="AR9" s="17"/>
-      <c r="AS9" s="17" cm="1">
+      <c r="AS9" s="17">
         <f t="array" ref="AS9">SUM(IF(ROUND(AR16:AR267,0)&lt;&gt;ROUND(AS16:AS267,0), 1, 0)) + COUNTBLANK(AR16:AR267) + COUNTIF(AR16:AR267, 0) - COUNTBLANK(AS16:AS267) - COUNTIF(AS16:AS267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AT9" s="17" cm="1">
+      <c r="AT9" s="17">
         <f t="array" ref="AT9">SUM(IF(ROUND(AR16:AR267,0)&lt;&gt;ROUND(AT16:AT267,0), 1, 0)) + COUNTBLANK(AR16:AR267) + COUNTIF(AR16:AR267, 0) - COUNTBLANK(AT16:AT267) - COUNTIF(AT16:AT267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AU9" s="17" cm="1">
+      <c r="AU9" s="17">
         <f t="array" ref="AU9">SUM(IF(ROUND(AR16:AR267,0)&lt;&gt;ROUND(AU16:AU267,0), 1, 0)) + COUNTBLANK(AR16:AR267) + COUNTIF(AR16:AR267, 0) - COUNTBLANK(AU16:AU267) - COUNTIF(AU16:AU267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AV9" s="17" cm="1">
+      <c r="AV9" s="17">
         <f t="array" ref="AV9">SUM(IF(ROUND(AR16:AR267,0)&lt;&gt;ROUND(AV16:AV267,0), 1, 0)) + COUNTBLANK(AR16:AR267) + COUNTIF(AR16:AR267, 0) - COUNTBLANK(AV16:AV267) - COUNTIF(AV16:AV267, 0)</f>
         <v>0</v>
       </c>
-      <c r="AW9" s="17" cm="1">
+      <c r="AW9" s="17">
         <f t="array" ref="AW9">SUM(IF(ROUND(AR16:AR267,0)&lt;&gt;ROUND(AW16:AW267,0), 1, 0)) + COUNTBLANK(AR16:AR267) + COUNTIF(AR16:AR267, 0) - COUNTBLANK(AW16:AW267) - COUNTIF(AW16:AW267, 0)</f>
         <v>0</v>
       </c>
       <c r="AY9" s="17"/>
-      <c r="AZ9" s="17" cm="1">
+      <c r="AZ9" s="17">
         <f t="array" ref="AZ9">SUM(IF(ROUND(AY16:AY267,0)&lt;&gt;ROUND(AZ16:AZ267,0), 1, 0)) + COUNTBLANK(AY16:AY267) + COUNTIF(AY16:AY267, 0) - COUNTBLANK(AZ16:AZ267) - COUNTIF(AZ16:AZ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BA9" s="17" cm="1">
+      <c r="BA9" s="17">
         <f t="array" ref="BA9">SUM(IF(ROUND(AY16:AY267,0)&lt;&gt;ROUND(BA16:BA267,0), 1, 0)) + COUNTBLANK(AY16:AY267) + COUNTIF(AY16:AY267, 0) - COUNTBLANK(BA16:BA267) - COUNTIF(BA16:BA267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BB9" s="17" cm="1">
+      <c r="BB9" s="17">
         <f t="array" ref="BB9">SUM(IF(ROUND(AY16:AY267,0)&lt;&gt;ROUND(BB16:BB267,0), 1, 0)) + COUNTBLANK(AY16:AY267) + COUNTIF(AY16:AY267, 0) - COUNTBLANK(BB16:BB267) - COUNTIF(BB16:BB267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BC9" s="17" cm="1">
+      <c r="BC9" s="17">
         <f t="array" ref="BC9">SUM(IF(ROUND(AY16:AY267,0)&lt;&gt;ROUND(BC16:BC267,0), 1, 0)) + COUNTBLANK(AY16:AY267) + COUNTIF(AY16:AY267, 0) - COUNTBLANK(BC16:BC267) - COUNTIF(BC16:BC267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BD9" s="17" cm="1">
+      <c r="BD9" s="17">
         <f t="array" ref="BD9">SUM(IF(ROUND(AY16:AY267,0)&lt;&gt;ROUND(BD16:BD267,0), 1, 0)) + COUNTBLANK(AY16:AY267) + COUNTIF(AY16:AY267, 0) - COUNTBLANK(BD16:BD267) - COUNTIF(BD16:BD267, 0)</f>
         <v>0</v>
       </c>
       <c r="BF9" s="17"/>
-      <c r="BG9" s="17" cm="1">
+      <c r="BG9" s="17">
         <f t="array" ref="BG9">SUM(IF(ROUND(BF16:BF267,0)&lt;&gt;ROUND(BG16:BG267,0), 1, 0)) + COUNTBLANK(BF16:BF267) + COUNTIF(BF16:BF267, 0) - COUNTBLANK(BG16:BG267) - COUNTIF(BG16:BG267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BH9" s="17" cm="1">
+      <c r="BH9" s="17">
         <f t="array" ref="BH9">SUM(IF(ROUND(BF16:BF267,0)&lt;&gt;ROUND(BH16:BH267,0), 1, 0)) + COUNTBLANK(BF16:BF267) + COUNTIF(BF16:BF267, 0) - COUNTBLANK(BH16:BH267) - COUNTIF(BH16:BH267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BI9" s="17" cm="1">
+      <c r="BI9" s="17">
         <f t="array" ref="BI9">SUM(IF(ROUND(BF16:BF267,0)&lt;&gt;ROUND(BI16:BI267,0), 1, 0)) + COUNTBLANK(BF16:BF267) + COUNTIF(BF16:BF267, 0) - COUNTBLANK(BI16:BI267) - COUNTIF(BI16:BI267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BJ9" s="17" cm="1">
+      <c r="BJ9" s="17">
         <f t="array" ref="BJ9">SUM(IF(ROUND(BF16:BF267,0)&lt;&gt;ROUND(BJ16:BJ267,0), 1, 0)) + COUNTBLANK(BF16:BF267) + COUNTIF(BF16:BF267, 0) - COUNTBLANK(BJ16:BJ267) - COUNTIF(BJ16:BJ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BK9" s="17" cm="1">
+      <c r="BK9" s="17">
         <f t="array" ref="BK9">SUM(IF(ROUND(BF16:BF267,0)&lt;&gt;ROUND(BK16:BK267,0), 1, 0)) + COUNTBLANK(BF16:BF267) + COUNTIF(BF16:BF267, 0) - COUNTBLANK(BK16:BK267) - COUNTIF(BK16:BK267, 0)</f>
         <v>0</v>
       </c>
       <c r="BM9" s="17"/>
-      <c r="BN9" s="17" cm="1">
+      <c r="BN9" s="17">
         <f t="array" ref="BN9">SUM(IF(ROUND(BM16:BM267,0)&lt;&gt;ROUND(BN16:BN267,0), 1, 0)) + COUNTBLANK(BM16:BM267) + COUNTIF(BM16:BM267, 0) - COUNTBLANK(BN16:BN267) - COUNTIF(BN16:BN267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BO9" s="17" cm="1">
+      <c r="BO9" s="17">
         <f t="array" ref="BO9">SUM(IF(ROUND(BM16:BM267,0)&lt;&gt;ROUND(BO16:BO267,0), 1, 0)) + COUNTBLANK(BM16:BM267) + COUNTIF(BM16:BM267, 0) - COUNTBLANK(BO16:BO267) - COUNTIF(BO16:BO267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BP9" s="17" cm="1">
+      <c r="BP9" s="17">
         <f t="array" ref="BP9">SUM(IF(ROUND(BM16:BM267,0)&lt;&gt;ROUND(BP16:BP267,0), 1, 0)) + COUNTBLANK(BM16:BM267) + COUNTIF(BM16:BM267, 0) - COUNTBLANK(BP16:BP267) - COUNTIF(BP16:BP267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BQ9" s="17" cm="1">
+      <c r="BQ9" s="17">
         <f t="array" ref="BQ9">SUM(IF(ROUND(BM16:BM267,0)&lt;&gt;ROUND(BQ16:BQ267,0), 1, 0)) + COUNTBLANK(BM16:BM267) + COUNTIF(BM16:BM267, 0) - COUNTBLANK(BQ16:BQ267) - COUNTIF(BQ16:BQ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BR9" s="17" cm="1">
+      <c r="BR9" s="17">
         <f t="array" ref="BR9">SUM(IF(ROUND(BM16:BM267,0)&lt;&gt;ROUND(BR16:BR267,0), 1, 0)) + COUNTBLANK(BM16:BM267) + COUNTIF(BM16:BM267, 0) - COUNTBLANK(BR16:BR267) - COUNTIF(BR16:BR267, 0)</f>
         <v>0</v>
       </c>
       <c r="BT9" s="17"/>
-      <c r="BU9" s="17" cm="1">
+      <c r="BU9" s="17">
         <f t="array" ref="BU9">SUM(IF(ROUND(BT16:BT267,0)&lt;&gt;ROUND(BU16:BU267,0), 1, 0)) + COUNTBLANK(BT16:BT267) + COUNTIF(BT16:BT267, 0) - COUNTBLANK(BU16:BU267) - COUNTIF(BU16:BU267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BV9" s="17" cm="1">
+      <c r="BV9" s="17">
         <f t="array" ref="BV9">SUM(IF(ROUND(BT16:BT267,0)&lt;&gt;ROUND(BV16:BV267,0), 1, 0)) + COUNTBLANK(BT16:BT267) + COUNTIF(BT16:BT267, 0) - COUNTBLANK(BV16:BV267) - COUNTIF(BV16:BV267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BW9" s="17" cm="1">
+      <c r="BW9" s="17">
         <f t="array" ref="BW9">SUM(IF(ROUND(BT16:BT267,0)&lt;&gt;ROUND(BW16:BW267,0), 1, 0)) + COUNTBLANK(BT16:BT267) + COUNTIF(BT16:BT267, 0) - COUNTBLANK(BW16:BW267) - COUNTIF(BW16:BW267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BX9" s="17" cm="1">
+      <c r="BX9" s="17">
         <f t="array" ref="BX9">SUM(IF(ROUND(BT16:BT267,0)&lt;&gt;ROUND(BX16:BX267,0), 1, 0)) + COUNTBLANK(BT16:BT267) + COUNTIF(BT16:BT267, 0) - COUNTBLANK(BX16:BX267) - COUNTIF(BX16:BX267, 0)</f>
         <v>0</v>
       </c>
-      <c r="BY9" s="17" cm="1">
+      <c r="BY9" s="17">
         <f t="array" ref="BY9">SUM(IF(ROUND(BT16:BT267,0)&lt;&gt;ROUND(BY16:BY267,0), 1, 0)) + COUNTBLANK(BT16:BT267) + COUNTIF(BT16:BT267, 0) - COUNTBLANK(BY16:BY267) - COUNTIF(BY16:BY267, 0)</f>
         <v>0</v>
       </c>
       <c r="CA9" s="17"/>
-      <c r="CB9" s="17" cm="1">
+      <c r="CB9" s="17">
         <f t="array" ref="CB9">SUM(IF(ROUND(CA16:CA267,0)&lt;&gt;ROUND(CB16:CB267,0), 1, 0)) + COUNTBLANK(CA16:CA267) + COUNTIF(CA16:CA267, 0) - COUNTBLANK(CB16:CB267) - COUNTIF(CB16:CB267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CC9" s="17" cm="1">
+      <c r="CC9" s="17">
         <f t="array" ref="CC9">SUM(IF(ROUND(CA16:CA267,0)&lt;&gt;ROUND(CC16:CC267,0), 1, 0)) + COUNTBLANK(CA16:CA267) + COUNTIF(CA16:CA267, 0) - COUNTBLANK(CC16:CC267) - COUNTIF(CC16:CC267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CD9" s="17" cm="1">
+      <c r="CD9" s="17">
         <f t="array" ref="CD9">SUM(IF(ROUND(CA16:CA267,0)&lt;&gt;ROUND(CD16:CD267,0), 1, 0)) + COUNTBLANK(CA16:CA267) + COUNTIF(CA16:CA267, 0) - COUNTBLANK(CD16:CD267) - COUNTIF(CD16:CD267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CE9" s="17" cm="1">
+      <c r="CE9" s="17">
         <f t="array" ref="CE9">SUM(IF(ROUND(CA16:CA267,0)&lt;&gt;ROUND(CE16:CE267,0), 1, 0)) + COUNTBLANK(CA16:CA267) + COUNTIF(CA16:CA267, 0) - COUNTBLANK(CE16:CE267) - COUNTIF(CE16:CE267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CF9" s="17" cm="1">
+      <c r="CF9" s="17">
         <f t="array" ref="CF9">SUM(IF(ROUND(CA16:CA267,0)&lt;&gt;ROUND(CF16:CF267,0), 1, 0)) + COUNTBLANK(CA16:CA267) + COUNTIF(CA16:CA267, 0) - COUNTBLANK(CF16:CF267) - COUNTIF(CF16:CF267, 0)</f>
         <v>0</v>
       </c>
       <c r="CH9" s="17"/>
-      <c r="CI9" s="17" cm="1">
+      <c r="CI9" s="17">
         <f t="array" ref="CI9">SUM(IF(ROUND(CH16:CH267,0)&lt;&gt;ROUND(CI16:CI267,0), 1, 0)) + COUNTBLANK(CH16:CH267) + COUNTIF(CH16:CH267, 0) - COUNTBLANK(CI16:CI267) - COUNTIF(CI16:CI267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CJ9" s="17" cm="1">
+      <c r="CJ9" s="17">
         <f t="array" ref="CJ9">SUM(IF(ROUND(CH16:CH267,0)&lt;&gt;ROUND(CJ16:CJ267,0), 1, 0)) + COUNTBLANK(CH16:CH267) + COUNTIF(CH16:CH267, 0) - COUNTBLANK(CJ16:CJ267) - COUNTIF(CJ16:CJ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CK9" s="17" cm="1">
+      <c r="CK9" s="17">
         <f t="array" ref="CK9">SUM(IF(ROUND(CH16:CH267,0)&lt;&gt;ROUND(CK16:CK267,0), 1, 0)) + COUNTBLANK(CH16:CH267) + COUNTIF(CH16:CH267, 0) - COUNTBLANK(CK16:CK267) - COUNTIF(CK16:CK267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CL9" s="17" cm="1">
+      <c r="CL9" s="17">
         <f t="array" ref="CL9">SUM(IF(ROUND(CH16:CH267,0)&lt;&gt;ROUND(CL16:CL267,0), 1, 0)) + COUNTBLANK(CH16:CH267) + COUNTIF(CH16:CH267, 0) - COUNTBLANK(CL16:CL267) - COUNTIF(CL16:CL267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CM9" s="17" cm="1">
+      <c r="CM9" s="17">
         <f t="array" ref="CM9">SUM(IF(ROUND(CH16:CH267,0)&lt;&gt;ROUND(CM16:CM267,0), 1, 0)) + COUNTBLANK(CH16:CH267) + COUNTIF(CH16:CH267, 0) - COUNTBLANK(CM16:CM267) - COUNTIF(CM16:CM267, 0)</f>
         <v>0</v>
       </c>
       <c r="CO9" s="17"/>
-      <c r="CP9" s="17" cm="1">
+      <c r="CP9" s="17">
         <f t="array" ref="CP9">SUM(IF(ROUND(CO16:CO267,0)&lt;&gt;ROUND(CP16:CP267,0), 1, 0)) + COUNTBLANK(CO16:CO267) + COUNTIF(CO16:CO267, 0) - COUNTBLANK(CP16:CP267) - COUNTIF(CP16:CP267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CQ9" s="17" cm="1">
+      <c r="CQ9" s="17">
         <f t="array" ref="CQ9">SUM(IF(ROUND(CO16:CO267,0)&lt;&gt;ROUND(CQ16:CQ267,0), 1, 0)) + COUNTBLANK(CO16:CO267) + COUNTIF(CO16:CO267, 0) - COUNTBLANK(CQ16:CQ267) - COUNTIF(CQ16:CQ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CR9" s="17" cm="1">
+      <c r="CR9" s="17">
         <f t="array" ref="CR9">SUM(IF(ROUND(CO16:CO267,0)&lt;&gt;ROUND(CR16:CR267,0), 1, 0)) + COUNTBLANK(CO16:CO267) + COUNTIF(CO16:CO267, 0) - COUNTBLANK(CR16:CR267) - COUNTIF(CR16:CR267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CS9" s="17" cm="1">
+      <c r="CS9" s="17">
         <f t="array" ref="CS9">SUM(IF(ROUND(CO16:CO267,0)&lt;&gt;ROUND(CS16:CS267,0), 1, 0)) + COUNTBLANK(CO16:CO267) + COUNTIF(CO16:CO267, 0) - COUNTBLANK(CS16:CS267) - COUNTIF(CS16:CS267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CT9" s="17" cm="1">
+      <c r="CT9" s="17">
         <f t="array" ref="CT9">SUM(IF(ROUND(CO16:CO267,0)&lt;&gt;ROUND(CT16:CT267,0), 1, 0)) + COUNTBLANK(CO16:CO267) + COUNTIF(CO16:CO267, 0) - COUNTBLANK(CT16:CT267) - COUNTIF(CT16:CT267, 0)</f>
         <v>0</v>
       </c>
       <c r="CV9" s="17"/>
-      <c r="CW9" s="17" cm="1">
+      <c r="CW9" s="17">
         <f t="array" ref="CW9">SUM(IF(ROUND(CV16:CV267,0)&lt;&gt;ROUND(CW16:CW267,0), 1, 0)) + COUNTBLANK(CV16:CV267) + COUNTIF(CV16:CV267, 0) - COUNTBLANK(CW16:CW267) - COUNTIF(CW16:CW267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CX9" s="17" cm="1">
+      <c r="CX9" s="17">
         <f t="array" ref="CX9">SUM(IF(ROUND(CV16:CV267,0)&lt;&gt;ROUND(CX16:CX267,0), 1, 0)) + COUNTBLANK(CV16:CV267) + COUNTIF(CV16:CV267, 0) - COUNTBLANK(CX16:CX267) - COUNTIF(CX16:CX267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CY9" s="17" cm="1">
+      <c r="CY9" s="17">
         <f t="array" ref="CY9">SUM(IF(ROUND(CV16:CV267,0)&lt;&gt;ROUND(CY16:CY267,0), 1, 0)) + COUNTBLANK(CV16:CV267) + COUNTIF(CV16:CV267, 0) - COUNTBLANK(CY16:CY267) - COUNTIF(CY16:CY267, 0)</f>
         <v>0</v>
       </c>
-      <c r="CZ9" s="17" cm="1">
+      <c r="CZ9" s="17">
         <f t="array" ref="CZ9">SUM(IF(ROUND(CV16:CV267,0)&lt;&gt;ROUND(CZ16:CZ267,0), 1, 0)) + COUNTBLANK(CV16:CV267) + COUNTIF(CV16:CV267, 0) - COUNTBLANK(CZ16:CZ267) - COUNTIF(CZ16:CZ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DA9" s="17" cm="1">
+      <c r="DA9" s="17">
         <f t="array" ref="DA9">SUM(IF(ROUND(CV16:CV267,0)&lt;&gt;ROUND(DA16:DA267,0), 1, 0)) + COUNTBLANK(CV16:CV267) + COUNTIF(CV16:CV267, 0) - COUNTBLANK(DA16:DA267) - COUNTIF(DA16:DA267, 0)</f>
         <v>0</v>
       </c>
       <c r="DC9" s="17"/>
-      <c r="DD9" s="17" cm="1">
-        <f t="array" ref="DD9">SUM(IF(ROUND(DC16:DC267,0)&lt;&gt;ROUND(DD16:DD267,0), 1, 0)) + COUNTBLANK(DC16:DC267) + COUNTIF(DC16:DC267, 0) - COUNTBLANK(DD16:DD267) - COUNTIF(DD16:DD267, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="DE9" s="17" cm="1">
-        <f t="array" ref="DE9">SUM(IF(ROUND(DC16:DC267,0)&lt;&gt;ROUND(DE16:DE267,0), 1, 0)) + COUNTBLANK(DC16:DC267) + COUNTIF(DC16:DC267, 0) - COUNTBLANK(DE16:DE267) - COUNTIF(DE16:DE267, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="DF9" s="17" cm="1">
-        <f t="array" ref="DF9">SUM(IF(ROUND(DC16:DC267,0)&lt;&gt;ROUND(DF16:DF267,0), 1, 0)) + COUNTBLANK(DC16:DC267) + COUNTIF(DC16:DC267, 0) - COUNTBLANK(DF16:DF267) - COUNTIF(DF16:DF267, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="DG9" s="17" cm="1">
-        <f t="array" ref="DG9">SUM(IF(ROUND(DC16:DC267,0)&lt;&gt;ROUND(DG16:DG267,0), 1, 0)) + COUNTBLANK(DC16:DC267) + COUNTIF(DC16:DC267, 0) - COUNTBLANK(DG16:DG267) - COUNTIF(DG16:DG267, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="DH9" s="17" cm="1">
-        <f t="array" ref="DH9">SUM(IF(ROUND(DC16:DC267,0)&lt;&gt;ROUND(DH16:DH267,0), 1, 0)) + COUNTBLANK(DC16:DC267) + COUNTIF(DC16:DC267, 0) - COUNTBLANK(DH16:DH267) - COUNTIF(DH16:DH267, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="DD9" s="17"/>
+      <c r="DE9" s="17"/>
+      <c r="DF9" s="17"/>
+      <c r="DG9" s="17"/>
+      <c r="DH9" s="17"/>
       <c r="DJ9" s="17"/>
-      <c r="DK9" s="17" cm="1">
+      <c r="DK9" s="17">
         <f t="array" ref="DK9">SUM(IF(ROUND(DJ16:DJ267,0)&lt;&gt;ROUND(DK16:DK267,0), 1, 0)) + COUNTBLANK(DJ16:DJ267) + COUNTIF(DJ16:DJ267, 0) - COUNTBLANK(DK16:DK267) - COUNTIF(DK16:DK267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DL9" s="17" cm="1">
+      <c r="DL9" s="17">
         <f t="array" ref="DL9">SUM(IF(ROUND(DJ16:DJ267,0)&lt;&gt;ROUND(DL16:DL267,0), 1, 0)) + COUNTBLANK(DJ16:DJ267) + COUNTIF(DJ16:DJ267, 0) - COUNTBLANK(DL16:DL267) - COUNTIF(DL16:DL267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DM9" s="17" cm="1">
+      <c r="DM9" s="17">
         <f t="array" ref="DM9">SUM(IF(ROUND(DJ16:DJ267,0)&lt;&gt;ROUND(DM16:DM267,0), 1, 0)) + COUNTBLANK(DJ16:DJ267) + COUNTIF(DJ16:DJ267, 0) - COUNTBLANK(DM16:DM267) - COUNTIF(DM16:DM267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DN9" s="17" cm="1">
+      <c r="DN9" s="17">
         <f t="array" ref="DN9">SUM(IF(ROUND(DJ16:DJ267,0)&lt;&gt;ROUND(DN16:DN267,0), 1, 0)) + COUNTBLANK(DJ16:DJ267) + COUNTIF(DJ16:DJ267, 0) - COUNTBLANK(DN16:DN267) - COUNTIF(DN16:DN267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DO9" s="17" cm="1">
+      <c r="DO9" s="17">
         <f t="array" ref="DO9">SUM(IF(ROUND(DJ16:DJ267,0)&lt;&gt;ROUND(DO16:DO267,0), 1, 0)) + COUNTBLANK(DJ16:DJ267) + COUNTIF(DJ16:DJ267, 0) - COUNTBLANK(DO16:DO267) - COUNTIF(DO16:DO267, 0)</f>
         <v>0</v>
       </c>
       <c r="DQ9" s="17"/>
-      <c r="DR9" s="17" cm="1">
+      <c r="DR9" s="17">
         <f t="array" ref="DR9">SUM(IF(ROUND(DQ16:DQ267,0)&lt;&gt;ROUND(DR16:DR267,0), 1, 0)) + COUNTBLANK(DQ16:DQ267) + COUNTIF(DQ16:DQ267, 0) - COUNTBLANK(DR16:DR267) - COUNTIF(DR16:DR267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DS9" s="17" cm="1">
+      <c r="DS9" s="17">
         <f t="array" ref="DS9">SUM(IF(ROUND(DQ16:DQ267,0)&lt;&gt;ROUND(DS16:DS267,0), 1, 0)) + COUNTBLANK(DQ16:DQ267) + COUNTIF(DQ16:DQ267, 0) - COUNTBLANK(DS16:DS267) - COUNTIF(DS16:DS267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DT9" s="17" cm="1">
+      <c r="DT9" s="17">
         <f t="array" ref="DT9">SUM(IF(ROUND(DQ16:DQ267,0)&lt;&gt;ROUND(DT16:DT267,0), 1, 0)) + COUNTBLANK(DQ16:DQ267) + COUNTIF(DQ16:DQ267, 0) - COUNTBLANK(DT16:DT267) - COUNTIF(DT16:DT267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DU9" s="17" cm="1">
+      <c r="DU9" s="17">
         <f t="array" ref="DU9">SUM(IF(ROUND(DQ16:DQ267,0)&lt;&gt;ROUND(DU16:DU267,0), 1, 0)) + COUNTBLANK(DQ16:DQ267) + COUNTIF(DQ16:DQ267, 0) - COUNTBLANK(DU16:DU267) - COUNTIF(DU16:DU267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DV9" s="17" cm="1">
+      <c r="DV9" s="17">
         <f t="array" ref="DV9">SUM(IF(ROUND(DQ16:DQ267,0)&lt;&gt;ROUND(DV16:DV267,0), 1, 0)) + COUNTBLANK(DQ16:DQ267) + COUNTIF(DQ16:DQ267, 0) - COUNTBLANK(DV16:DV267) - COUNTIF(DV16:DV267, 0)</f>
         <v>0</v>
       </c>
       <c r="DX9" s="17"/>
-      <c r="DY9" s="17" cm="1">
+      <c r="DY9" s="17">
         <f t="array" ref="DY9">SUM(IF(ROUND(DX16:DX267,0)&lt;&gt;ROUND(DY16:DY267,0), 1, 0)) + COUNTBLANK(DX16:DX267) + COUNTIF(DX16:DX267, 0) - COUNTBLANK(DY16:DY267) - COUNTIF(DY16:DY267, 0)</f>
         <v>0</v>
       </c>
-      <c r="DZ9" s="17" cm="1">
+      <c r="DZ9" s="17">
         <f t="array" ref="DZ9">SUM(IF(ROUND(DX16:DX267,0)&lt;&gt;ROUND(DZ16:DZ267,0), 1, 0)) + COUNTBLANK(DX16:DX267) + COUNTIF(DX16:DX267, 0) - COUNTBLANK(DZ16:DZ267) - COUNTIF(DZ16:DZ267, 0)</f>
         <v>0</v>
       </c>
-      <c r="EA9" s="17" cm="1">
+      <c r="EA9" s="17">
         <f t="array" ref="EA9">SUM(IF(ROUND(DX16:DX267,0)&lt;&gt;ROUND(EA16:EA267,0), 1, 0)) + COUNTBLANK(DX16:DX267) + COUNTIF(DX16:DX267, 0) - COUNTBLANK(EA16:EA267) - COUNTIF(EA16:EA267, 0)</f>
         <v>0</v>
       </c>
-      <c r="EB9" s="17" cm="1">
+      <c r="EB9" s="17">
         <f t="array" ref="EB9">SUM(IF(ROUND(DX16:DX267,0)&lt;&gt;ROUND(EB16:EB267,0), 1, 0)) + COUNTBLANK(DX16:DX267) + COUNTIF(DX16:DX267, 0) - COUNTBLANK(EB16:EB267) - COUNTIF(EB16:EB267, 0)</f>
         <v>0</v>
       </c>
-      <c r="EC9" s="17" cm="1">
+      <c r="EC9" s="17">
         <f t="array" ref="EC9">SUM(IF(ROUND(DX16:DX267,0)&lt;&gt;ROUND(EC16:EC267,0), 1, 0)) + COUNTBLANK(DX16:DX267) + COUNTIF(DX16:DX267, 0) - COUNTBLANK(EC16:EC267) - COUNTIF(EC16:EC267, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:138" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="57"/>
+      <c r="G10" s="44"/>
+      <c r="I10" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="G10" s="56"/>
-      <c r="H10"/>
-      <c r="I10" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="45"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10"/>
-      <c r="AW10"/>
-      <c r="AY10"/>
-      <c r="AZ10"/>
-      <c r="BA10"/>
-      <c r="BB10"/>
-      <c r="BC10"/>
-      <c r="BD10"/>
-      <c r="BF10"/>
-      <c r="BG10"/>
-      <c r="BH10"/>
-      <c r="BI10"/>
-      <c r="BJ10"/>
-      <c r="BK10"/>
-      <c r="BM10"/>
-      <c r="BN10"/>
-      <c r="BO10"/>
-      <c r="BP10"/>
-      <c r="BQ10"/>
-      <c r="BR10"/>
-      <c r="BT10"/>
-      <c r="BU10"/>
-      <c r="BV10"/>
-      <c r="BW10"/>
-      <c r="BX10"/>
-      <c r="BY10"/>
-      <c r="CA10"/>
-      <c r="CB10"/>
-      <c r="CC10"/>
-      <c r="CD10"/>
-      <c r="CE10"/>
-      <c r="CF10"/>
-      <c r="CH10"/>
-      <c r="CI10"/>
-      <c r="CJ10"/>
-      <c r="CK10"/>
-      <c r="CL10"/>
-      <c r="CM10"/>
-      <c r="CO10"/>
-      <c r="CP10"/>
-      <c r="CQ10"/>
-      <c r="CR10"/>
-      <c r="CS10"/>
-      <c r="CT10"/>
-      <c r="CV10"/>
-      <c r="CW10"/>
-      <c r="CX10"/>
-      <c r="CY10"/>
-      <c r="CZ10"/>
-      <c r="DA10"/>
-      <c r="DC10"/>
-      <c r="DD10"/>
-      <c r="DE10"/>
-      <c r="DF10"/>
-      <c r="DG10"/>
-      <c r="DH10"/>
-      <c r="DJ10"/>
-      <c r="DK10"/>
-      <c r="DL10"/>
-      <c r="DM10"/>
-      <c r="DN10"/>
-      <c r="DO10"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="46"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="41"/>
     </row>
     <row r="12" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A12" s="17"/>
-      <c r="B12" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="44"/>
-      <c r="I12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="Q12" s="58" t="s">
+      <c r="B12" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="59"/>
-      <c r="S12" s="60"/>
-      <c r="X12" s="38" t="s">
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="17"/>
+      <c r="I12" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="39"/>
-      <c r="Z12" s="40"/>
-      <c r="AE12" s="38" t="s">
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="17"/>
+      <c r="Q12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AF12" s="38"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="53"/>
+      <c r="X12" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y12" s="55"/>
+      <c r="Z12" s="53"/>
+      <c r="AE12" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF12" s="53"/>
       <c r="AG12" s="36"/>
       <c r="AH12" s="37"/>
-      <c r="AK12" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL12" s="62"/>
-      <c r="AM12" s="49"/>
-      <c r="AN12" s="49"/>
-      <c r="AO12" s="45"/>
-      <c r="AR12" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS12" s="49"/>
-      <c r="AT12" s="49"/>
-      <c r="AU12" s="49"/>
-      <c r="AV12" s="45"/>
-      <c r="AY12" s="44" t="s">
+      <c r="AK12" s="45"/>
+      <c r="AL12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AZ12" s="49"/>
-      <c r="BA12" s="49"/>
-      <c r="BB12" s="49"/>
-      <c r="BC12" s="45"/>
-      <c r="BF12" s="44" t="s">
+      <c r="AM12" s="36"/>
+      <c r="AN12" s="36"/>
+      <c r="AO12" s="37"/>
+      <c r="AS12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="BG12" s="49"/>
-      <c r="BH12" s="49"/>
-      <c r="BI12" s="49"/>
-      <c r="BJ12" s="45"/>
-      <c r="BM12" s="44" t="s">
+      <c r="AT12" s="36"/>
+      <c r="AU12" s="36"/>
+      <c r="AV12" s="37"/>
+      <c r="AY12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="BN12" s="49"/>
-      <c r="BO12" s="49"/>
-      <c r="BP12" s="49"/>
-      <c r="BQ12" s="45"/>
-      <c r="BT12" s="44" t="s">
+      <c r="AZ12" s="36"/>
+      <c r="BA12" s="36"/>
+      <c r="BB12" s="36"/>
+      <c r="BC12" s="37"/>
+      <c r="BF12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="BU12" s="49"/>
-      <c r="BV12" s="49"/>
-      <c r="BW12" s="49"/>
-      <c r="BX12" s="45"/>
-      <c r="CA12" s="44" t="s">
+      <c r="BG12" s="36"/>
+      <c r="BH12" s="36"/>
+      <c r="BI12" s="36"/>
+      <c r="BJ12" s="37"/>
+      <c r="BM12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="CB12" s="49"/>
-      <c r="CC12" s="49"/>
-      <c r="CD12" s="49"/>
-      <c r="CE12" s="45"/>
-      <c r="CH12" s="44" t="s">
+      <c r="BN12" s="36"/>
+      <c r="BO12" s="36"/>
+      <c r="BP12" s="36"/>
+      <c r="BQ12" s="37"/>
+      <c r="BT12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="CI12" s="49"/>
-      <c r="CJ12" s="49"/>
-      <c r="CK12" s="49"/>
-      <c r="CL12" s="45"/>
-      <c r="CO12" s="44" t="s">
+      <c r="BU12" s="36"/>
+      <c r="BV12" s="36"/>
+      <c r="BW12" s="36"/>
+      <c r="BX12" s="37"/>
+      <c r="CA12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="CP12" s="49"/>
-      <c r="CQ12" s="49"/>
-      <c r="CR12" s="49"/>
-      <c r="CS12" s="45"/>
-      <c r="CV12" s="44" t="s">
+      <c r="CB12" s="36"/>
+      <c r="CC12" s="36"/>
+      <c r="CD12" s="36"/>
+      <c r="CE12" s="37"/>
+      <c r="CH12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="CW12" s="49"/>
-      <c r="CX12" s="49"/>
-      <c r="CY12" s="49"/>
-      <c r="CZ12" s="45"/>
-      <c r="DC12" s="44" t="s">
+      <c r="CI12" s="36"/>
+      <c r="CJ12" s="36"/>
+      <c r="CK12" s="36"/>
+      <c r="CL12" s="37"/>
+      <c r="CO12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="DD12" s="49"/>
-      <c r="DE12" s="49"/>
-      <c r="DF12" s="49"/>
-      <c r="DG12" s="45"/>
-      <c r="DJ12" s="44" t="s">
+      <c r="CP12" s="36"/>
+      <c r="CQ12" s="36"/>
+      <c r="CR12" s="36"/>
+      <c r="CS12" s="37"/>
+      <c r="CV12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="DK12" s="49"/>
-      <c r="DL12" s="49"/>
-      <c r="DM12" s="49"/>
-      <c r="DN12" s="45"/>
-      <c r="DQ12" s="44" t="s">
+      <c r="CW12" s="36"/>
+      <c r="CX12" s="36"/>
+      <c r="CY12" s="36"/>
+      <c r="CZ12" s="37"/>
+      <c r="DC12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="DX12" s="44" t="s">
+      <c r="DD12" s="36"/>
+      <c r="DE12" s="36"/>
+      <c r="DF12" s="36"/>
+      <c r="DG12" s="37"/>
+      <c r="DJ12" s="17" t="s">
         <v>28</v>
       </c>
+      <c r="DK12" s="36"/>
+      <c r="DL12" s="36"/>
+      <c r="DM12" s="36"/>
+      <c r="DN12" s="37"/>
+      <c r="DQ12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="DX12" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="13" spans="1:138" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="51"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="50"/>
-      <c r="AB13" s="50"/>
-      <c r="AE13" s="50"/>
-      <c r="AF13" s="50"/>
-      <c r="AG13" s="50"/>
-      <c r="AH13" s="50"/>
-      <c r="AI13" s="50"/>
-      <c r="AK13" s="50"/>
-      <c r="AL13" s="50"/>
-      <c r="AM13" s="50"/>
-      <c r="AN13" s="50"/>
-      <c r="AO13" s="50"/>
-      <c r="AR13" s="50"/>
-      <c r="AS13" s="50"/>
-      <c r="AT13" s="50"/>
-      <c r="AU13" s="50"/>
-      <c r="AV13" s="50"/>
-      <c r="AY13" s="50"/>
-      <c r="AZ13" s="50"/>
-      <c r="BA13" s="50"/>
-      <c r="BB13" s="50"/>
-      <c r="BC13" s="50"/>
-      <c r="BF13" s="50"/>
-      <c r="BG13" s="50"/>
-      <c r="BH13" s="50"/>
-      <c r="BI13" s="50"/>
-      <c r="BJ13" s="50"/>
-      <c r="BM13" s="50"/>
-      <c r="BN13" s="50"/>
-      <c r="BO13" s="50"/>
-      <c r="BP13" s="50"/>
-      <c r="BQ13" s="50"/>
-      <c r="BT13" s="50"/>
-      <c r="BU13" s="50"/>
-      <c r="BV13" s="50"/>
-      <c r="BW13" s="50"/>
-      <c r="BX13" s="50"/>
-      <c r="CA13" s="50"/>
-      <c r="CB13" s="50"/>
-      <c r="CC13" s="50"/>
-      <c r="CD13" s="50"/>
-      <c r="CE13" s="50"/>
-      <c r="CH13" s="50"/>
-      <c r="CI13" s="50"/>
-      <c r="CJ13" s="50"/>
-      <c r="CK13" s="50"/>
-      <c r="CL13" s="50"/>
-      <c r="CO13" s="50"/>
-      <c r="CP13" s="50"/>
-      <c r="CQ13" s="50"/>
-      <c r="CR13" s="50"/>
-      <c r="CS13" s="50"/>
-      <c r="CV13" s="50"/>
-      <c r="CW13" s="50"/>
-      <c r="CX13" s="50"/>
-      <c r="CY13" s="50"/>
-      <c r="CZ13" s="50"/>
-      <c r="DC13" s="50"/>
-      <c r="DD13" s="50"/>
-      <c r="DE13" s="50"/>
-      <c r="DF13" s="50"/>
-      <c r="DG13" s="50"/>
-      <c r="DJ13" s="50"/>
-      <c r="DK13" s="50"/>
-      <c r="DL13" s="50"/>
-      <c r="DM13" s="50"/>
-      <c r="DN13" s="50"/>
-      <c r="DQ13" s="50"/>
-      <c r="DR13" s="50"/>
-      <c r="DS13" s="50"/>
-      <c r="DT13" s="50"/>
-      <c r="DU13" s="50"/>
-      <c r="DX13" s="50"/>
-      <c r="DY13" s="50"/>
-      <c r="DZ13" s="50"/>
-      <c r="EA13" s="50"/>
-      <c r="EB13" s="50"/>
+    <row r="13" spans="1:138" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="42"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="T13" s="46"/>
+      <c r="U13" s="47"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
+      <c r="AE13" s="41"/>
+      <c r="AF13" s="41"/>
+      <c r="AG13" s="41"/>
+      <c r="AH13" s="41"/>
+      <c r="AI13" s="41"/>
+      <c r="AL13" s="41"/>
+      <c r="AM13" s="41"/>
+      <c r="AN13" s="41"/>
+      <c r="AO13" s="41"/>
+      <c r="AP13" s="41"/>
+      <c r="AS13" s="41"/>
+      <c r="AT13" s="41"/>
+      <c r="AU13" s="41"/>
+      <c r="AV13" s="41"/>
+      <c r="AW13" s="41"/>
+      <c r="AZ13" s="41"/>
+      <c r="BA13" s="41"/>
+      <c r="BB13" s="41"/>
+      <c r="BC13" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD13" s="41"/>
+      <c r="BE13" s="37"/>
+      <c r="BG13" s="46"/>
+      <c r="BH13" s="47"/>
+      <c r="BI13" s="41"/>
+      <c r="BJ13" s="41"/>
+      <c r="BK13" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="BN13" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO13" s="47"/>
+      <c r="BP13" s="41"/>
+      <c r="BQ13" s="41"/>
+      <c r="BR13" s="41"/>
+      <c r="BU13" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="BV13" s="41"/>
+      <c r="BW13" s="41"/>
+      <c r="BX13" s="41"/>
+      <c r="BY13" s="41"/>
+      <c r="CB13" s="41"/>
+      <c r="CC13" s="41"/>
+      <c r="CD13" s="41"/>
+      <c r="CE13" s="41"/>
+      <c r="CF13" s="41"/>
+      <c r="CI13" s="41"/>
+      <c r="CJ13" s="41"/>
+      <c r="CK13" s="41"/>
+      <c r="CL13" s="41"/>
+      <c r="CM13" s="41"/>
+      <c r="CP13" s="41"/>
+      <c r="CQ13" s="41"/>
+      <c r="CR13" s="41"/>
+      <c r="CS13" s="41"/>
+      <c r="CT13" s="41"/>
+      <c r="CW13" s="41"/>
+      <c r="CX13" s="41"/>
+      <c r="CY13" s="41"/>
+      <c r="CZ13" s="41"/>
+      <c r="DA13" s="41"/>
+      <c r="DD13" s="41"/>
+      <c r="DE13" s="41"/>
+      <c r="DF13" s="41"/>
+      <c r="DG13" s="41"/>
+      <c r="DH13" s="41"/>
+      <c r="DK13" s="41"/>
+      <c r="DL13" s="41"/>
+      <c r="DM13" s="41"/>
+      <c r="DN13" s="41"/>
+      <c r="DO13" s="41"/>
+      <c r="DR13" s="41"/>
+      <c r="DS13" s="41"/>
+      <c r="DT13" s="41"/>
+      <c r="DU13" s="41"/>
+      <c r="DV13" s="49"/>
+      <c r="DY13" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="DZ13" s="41"/>
+      <c r="EA13" s="41"/>
+      <c r="EB13" s="41"/>
     </row>
     <row r="14" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A14" s="29" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
@@ -2138,7 +2081,7 @@
       <c r="DN14" s="5"/>
       <c r="DO14" s="5"/>
       <c r="DP14" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="DQ14" s="5"/>
       <c r="DR14" s="5"/>
@@ -2154,7 +2097,7 @@
       <c r="EB14" s="5"/>
       <c r="EC14" s="5"/>
       <c r="ED14" s="4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="EE14" s="5"/>
       <c r="EF14" s="5"/>
@@ -2162,416 +2105,416 @@
     </row>
     <row r="15" spans="1:138" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="25" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="R15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="S15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="U15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="V15" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="W15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="X15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC15" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX15" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE15" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="BH15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="BJ15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="BK15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BL15" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="BM15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="BO15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="BP15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="BQ15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="BR15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BS15" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="BT15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="BV15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="BW15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="BX15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="BY15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="BZ15" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="CA15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="CB15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="CC15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="CD15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="CE15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="CF15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="CG15" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="CH15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="CI15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="CJ15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="CK15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="CL15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="CM15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="CN15" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="26" t="s">
-        <v>34</v>
+      <c r="CO15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>35</v>
+      <c r="CP15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="J15" s="26" t="s">
-        <v>58</v>
+      <c r="CQ15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="K15" s="26" t="s">
-        <v>59</v>
+      <c r="CR15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="L15" s="26" t="s">
-        <v>60</v>
+      <c r="CS15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="M15" s="26" t="s">
-        <v>61</v>
+      <c r="CT15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="N15" s="30" t="s">
-        <v>62</v>
+      <c r="CU15" s="25" t="s">
+        <v>63</v>
       </c>
-      <c r="O15" s="33" t="s">
-        <v>36</v>
+      <c r="CV15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="P15" s="26" t="s">
-        <v>35</v>
+      <c r="CW15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="Q15" s="26" t="s">
-        <v>58</v>
+      <c r="CX15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="R15" s="26" t="s">
-        <v>59</v>
+      <c r="CY15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="S15" s="26" t="s">
-        <v>60</v>
+      <c r="CZ15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="T15" s="26" t="s">
-        <v>61</v>
+      <c r="DA15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="U15" s="30" t="s">
-        <v>62</v>
+      <c r="DB15" s="25" t="s">
+        <v>64</v>
       </c>
-      <c r="V15" s="25" t="s">
-        <v>37</v>
+      <c r="DC15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="W15" s="26" t="s">
-        <v>35</v>
+      <c r="DD15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="X15" s="26" t="s">
-        <v>58</v>
+      <c r="DE15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="Y15" s="26" t="s">
-        <v>59</v>
+      <c r="DF15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="Z15" s="26" t="s">
-        <v>60</v>
+      <c r="DG15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="AA15" s="26" t="s">
-        <v>61</v>
+      <c r="DH15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="AB15" s="30" t="s">
-        <v>62</v>
+      <c r="DI15" s="4" t="s">
+        <v>65</v>
       </c>
-      <c r="AC15" s="25" t="s">
-        <v>38</v>
+      <c r="DJ15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="AD15" s="26" t="s">
-        <v>35</v>
+      <c r="DK15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="AE15" s="26" t="s">
-        <v>58</v>
+      <c r="DL15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="AF15" s="26" t="s">
-        <v>59</v>
+      <c r="DM15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="AG15" s="26" t="s">
-        <v>60</v>
+      <c r="DN15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="AH15" s="26" t="s">
-        <v>61</v>
+      <c r="DO15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="AI15" s="30" t="s">
-        <v>62</v>
+      <c r="DP15" s="4" t="s">
+        <v>66</v>
       </c>
-      <c r="AJ15" s="25" t="s">
-        <v>39</v>
+      <c r="DQ15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="AK15" s="26" t="s">
-        <v>35</v>
+      <c r="DR15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="AL15" s="26" t="s">
-        <v>58</v>
+      <c r="DS15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="AM15" s="26" t="s">
-        <v>59</v>
+      <c r="DT15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="AN15" s="26" t="s">
-        <v>60</v>
+      <c r="DU15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="AO15" s="26" t="s">
-        <v>61</v>
+      <c r="DV15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="AP15" s="30" t="s">
-        <v>62</v>
+      <c r="DW15" s="4" t="s">
+        <v>67</v>
       </c>
-      <c r="AQ15" s="25" t="s">
-        <v>40</v>
+      <c r="DX15" s="26" t="s">
+        <v>50</v>
       </c>
-      <c r="AR15" s="26" t="s">
-        <v>35</v>
+      <c r="DY15" s="26" t="s">
+        <v>44</v>
       </c>
-      <c r="AS15" s="26" t="s">
-        <v>58</v>
+      <c r="DZ15" s="26" t="s">
+        <v>45</v>
       </c>
-      <c r="AT15" s="26" t="s">
-        <v>59</v>
+      <c r="EA15" s="26" t="s">
+        <v>46</v>
       </c>
-      <c r="AU15" s="26" t="s">
-        <v>60</v>
+      <c r="EB15" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="AV15" s="26" t="s">
-        <v>61</v>
+      <c r="EC15" s="30" t="s">
+        <v>48</v>
       </c>
-      <c r="AW15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX15" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="AZ15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="BC15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="BD15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="BE15" s="25" t="s">
+      <c r="ED15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BF15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="BG15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL15" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="BM15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="BN15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="BO15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="BP15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="BQ15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="BR15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="BS15" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="BT15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="BU15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="BV15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="BW15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="BY15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="BZ15" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="CA15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="CB15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="CC15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="CD15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="CE15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="CF15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="CG15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="CH15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="CI15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="CJ15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="CK15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="CL15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="CM15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="CN15" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="CO15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="CP15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="CQ15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="CR15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="CS15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="CT15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="CU15" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="CV15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="CW15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="CX15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="CY15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="CZ15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="DA15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="DB15" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="DC15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="DD15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="DE15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="DF15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="DG15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="DH15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="DI15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="DJ15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="DK15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="DL15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="DM15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="DN15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="DO15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="DP15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="DQ15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="DR15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="DS15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="DT15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="DU15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="DV15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="DW15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="DX15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="DY15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="DZ15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="EA15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="EB15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="EC15" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="ED15" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="EE15" s="4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="EF15" s="4"/>
       <c r="EG15" s="4"/>
     </row>
     <row r="16" spans="1:138" x14ac:dyDescent="0.45">
       <c r="A16" s="27" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -2580,7 +2523,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="31" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="34"/>
@@ -2589,7 +2532,7 @@
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="P16" s="21"/>
       <c r="Q16" s="21"/>
@@ -2695,7 +2638,7 @@
       <c r="EB16" s="6"/>
       <c r="EC16" s="6"/>
       <c r="ED16" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="EE16" s="12"/>
       <c r="EF16" s="1"/>
@@ -2922,7 +2865,7 @@
       <c r="CZ18" s="35"/>
       <c r="DA18" s="35"/>
       <c r="DC18" s="6"/>
-      <c r="DD18" s="10"/>
+      <c r="DD18" s="6"/>
       <c r="DE18" s="10"/>
       <c r="DF18" s="10"/>
       <c r="DG18" s="6"/>
@@ -3325,7 +3268,7 @@
       <c r="EB21" s="6"/>
       <c r="EC21" s="6"/>
       <c r="ED21" s="3"/>
-      <c r="EE21" s="12"/>
+      <c r="EE21" s="51"/>
       <c r="EF21" s="1"/>
       <c r="EG21" s="1"/>
       <c r="EH21" s="1"/>
@@ -3451,7 +3394,7 @@
       <c r="EB22" s="6"/>
       <c r="EC22" s="6"/>
       <c r="ED22" s="3"/>
-      <c r="EE22" s="12"/>
+      <c r="EE22" s="51"/>
       <c r="EF22" s="1"/>
       <c r="EG22" s="1"/>
       <c r="EH22" s="1"/>
@@ -3589,7 +3532,7 @@
       <c r="EB23" s="6"/>
       <c r="EC23" s="6"/>
       <c r="ED23" s="3"/>
-      <c r="EE23" s="12"/>
+      <c r="EE23" s="51"/>
       <c r="EF23" s="1"/>
       <c r="EG23" s="1"/>
       <c r="EH23" s="1"/>
@@ -3715,7 +3658,7 @@
       <c r="EB24" s="6"/>
       <c r="EC24" s="6"/>
       <c r="ED24" s="3"/>
-      <c r="EE24" s="12"/>
+      <c r="EE24" s="51"/>
       <c r="EF24" s="1"/>
       <c r="EG24" s="1"/>
       <c r="EH24" s="1"/>
@@ -3841,7 +3784,7 @@
       <c r="EB25" s="6"/>
       <c r="EC25" s="6"/>
       <c r="ED25" s="3"/>
-      <c r="EE25" s="12"/>
+      <c r="EE25" s="51"/>
       <c r="EF25" s="1"/>
       <c r="EG25" s="1"/>
       <c r="EH25" s="1"/>
@@ -3967,7 +3910,7 @@
       <c r="EB26" s="6"/>
       <c r="EC26" s="6"/>
       <c r="ED26" s="3"/>
-      <c r="EE26" s="12"/>
+      <c r="EE26" s="51"/>
       <c r="EF26" s="1"/>
       <c r="EG26" s="1"/>
       <c r="EH26" s="1"/>
@@ -4092,7 +4035,7 @@
       <c r="EA27" s="10"/>
       <c r="EB27" s="6"/>
       <c r="EC27" s="6"/>
-      <c r="EE27" s="12"/>
+      <c r="EE27" s="51"/>
       <c r="EF27" s="1"/>
       <c r="EG27" s="1"/>
       <c r="EH27" s="1"/>
@@ -4217,7 +4160,7 @@
       <c r="EA28" s="10"/>
       <c r="EB28" s="6"/>
       <c r="EC28" s="6"/>
-      <c r="EE28" s="12"/>
+      <c r="EE28" s="51"/>
       <c r="EF28" s="1"/>
       <c r="EG28" s="1"/>
       <c r="EH28" s="1"/>
@@ -4342,7 +4285,7 @@
       <c r="EA29" s="10"/>
       <c r="EB29" s="6"/>
       <c r="EC29" s="6"/>
-      <c r="EE29" s="12"/>
+      <c r="EE29" s="51"/>
       <c r="EF29" s="1"/>
       <c r="EG29" s="1"/>
       <c r="EH29" s="1"/>
@@ -34098,109 +34041,112 @@
       <c r="EH267" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="J6:L6"/>
+  <mergeCells count="8">
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="I12:K12"/>
     <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
-  <conditionalFormatting sqref="C16:C267 J16:L267 R16:S267 Y16:Z267 AF16:AG267">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>AND(NOT(ISBLANK(C16)), ROUND(C16, 0) &lt;&gt; ROUND(B16, 0))</formula>
+  <conditionalFormatting sqref="C16:C267 G16:G267">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>AND(NOT(ISBLANK(C16)), ROUND(C16, 0) &lt;&gt; ROUND($B16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q16:Q267">
-    <cfRule type="expression" dxfId="16" priority="1">
-      <formula>AND(NOT(ISBLANK(Q16)), ROUND(Q16, 0) &lt;&gt; ROUND(P16, 0))</formula>
+  <conditionalFormatting sqref="J16:N267">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>AND(NOT(ISBLANK(J16)), ROUND(J16, 0) &lt;&gt; ROUND($I16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X16:X267">
-    <cfRule type="expression" dxfId="15" priority="17">
-      <formula>AND(NOT(ISBLANK(X16)), ROUND(X16, 0) &lt;&gt; ROUND(W16, 0))</formula>
+  <conditionalFormatting sqref="Q16:U267">
+    <cfRule type="expression" dxfId="16" priority="2">
+      <formula>AND(NOT(ISBLANK(Q16)), ROUND(Q16, 0) &lt;&gt; ROUND($P16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE16:AE267">
-    <cfRule type="expression" dxfId="14" priority="16">
-      <formula>AND(NOT(ISBLANK(AE16)), ROUND(AE16, 0) &lt;&gt; ROUND(AD16, 0))</formula>
+  <conditionalFormatting sqref="X16:AB267">
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>AND(NOT(ISBLANK(X16)), ROUND(X16, 0) &lt;&gt; ROUND($W16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL16:AN267">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>AND(NOT(ISBLANK(AL16)), ROUND(AL16, 0) &lt;&gt; ROUND(AK16, 0))</formula>
+  <conditionalFormatting sqref="AE16:AI267">
+    <cfRule type="expression" dxfId="14" priority="17">
+      <formula>AND(NOT(ISBLANK(AE16)), ROUND(AE16, 0) &lt;&gt; ROUND($AD16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS16:AU267">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>AND(NOT(ISBLANK(AS16)), ROUND(AS16, 0) &lt;&gt; ROUND(AR16, 0))</formula>
+  <conditionalFormatting sqref="AL16:AP267">
+    <cfRule type="expression" dxfId="13" priority="16">
+      <formula>AND(NOT(ISBLANK(AL16)), ROUND(AL16, 0) &lt;&gt; ROUND($AK16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ16:BB267">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>AND(NOT(ISBLANK(AZ16)), ROUND(AZ16, 0) &lt;&gt; ROUND(AY16, 0))</formula>
+  <conditionalFormatting sqref="AS16:AW267">
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>AND(NOT(ISBLANK(AS16)), ROUND(AS16, 0) &lt;&gt; ROUND($AR16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG16:BI267">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>AND(NOT(ISBLANK(BG16)), ROUND(BG16, 0) &lt;&gt; ROUND(BF16, 0))</formula>
+  <conditionalFormatting sqref="AZ16:BD267">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>AND(NOT(ISBLANK(AZ16)), ROUND(AZ16, 0) &lt;&gt; ROUND($AY16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN16:BP267">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>AND(NOT(ISBLANK(BN16)), ROUND(BN16, 0) &lt;&gt; ROUND(BM16, 0))</formula>
+  <conditionalFormatting sqref="BG16:BK267">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>AND(NOT(ISBLANK(BG16)), ROUND(BG16, 0) &lt;&gt; ROUND($BF16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BU16:BW267">
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>AND(NOT(ISBLANK(BU16)), ROUND(BU16, 0) &lt;&gt; ROUND(BT16, 0))</formula>
+  <conditionalFormatting sqref="BN16:BR267">
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>AND(NOT(ISBLANK(BN16)), ROUND(BN16, 0) &lt;&gt; ROUND($BM16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CB16:CD267">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>AND(NOT(ISBLANK(CB16)), ROUND(CB16, 0) &lt;&gt; ROUND(CA16, 0))</formula>
+  <conditionalFormatting sqref="BU16:BY267">
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>AND(NOT(ISBLANK(BU16)), ROUND(BU16, 0) &lt;&gt; ROUND($BT16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CI16:CK267">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>AND(NOT(ISBLANK(CI16)), ROUND(CI16, 0) &lt;&gt; ROUND(CH16, 0))</formula>
+  <conditionalFormatting sqref="CB16:CF267">
+    <cfRule type="expression" dxfId="7" priority="10">
+      <formula>AND(NOT(ISBLANK(CB16)), ROUND(CB16, 0) &lt;&gt; ROUND($CA16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CP16:CR267">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>AND(NOT(ISBLANK(CP16)), ROUND(CP16, 0) &lt;&gt; ROUND(CO16, 0))</formula>
+  <conditionalFormatting sqref="CI16:CM267">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>AND(NOT(ISBLANK(CI16)), ROUND(CI16, 0) &lt;&gt; ROUND($CH16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CW16:CY267">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>AND(NOT(ISBLANK(CW16)), ROUND(CW16, 0) &lt;&gt; ROUND(CV16, 0))</formula>
+  <conditionalFormatting sqref="CP16:CT267">
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>AND(NOT(ISBLANK(CP16)), ROUND(CP16, 0) &lt;&gt; ROUND($CO16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DD16:DF267">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>AND(NOT(ISBLANK(DD16)), ROUND(DD16, 0) &lt;&gt; ROUND(DC16, 0))</formula>
+  <conditionalFormatting sqref="CW16:DA267">
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>AND(NOT(ISBLANK(CW16)), ROUND(CW16, 0) &lt;&gt; ROUND($CV16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DK16:DM267">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(NOT(ISBLANK(DK16)), ROUND(DK16, 0) &lt;&gt; ROUND(DJ16, 0))</formula>
+  <conditionalFormatting sqref="DD16:DF17 DE18:DF18 DD19:DF267">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>AND(NOT(ISBLANK(DD16)), ROUND(DD16, 0) &lt;&gt; ROUND($DC16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DR16:DT267">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>AND(NOT(ISBLANK(DR16)), ROUND(DR16, 0) &lt;&gt; ROUND(DQ16, 0))</formula>
+  <conditionalFormatting sqref="DK16:DO267">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND(NOT(ISBLANK(DK16)), ROUND(DK16, 0) &lt;&gt; ROUND($DJ16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DY16:EA267">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(NOT(ISBLANK(DY16)), ROUND(DY16, 0) &lt;&gt; ROUND(DX16, 0))</formula>
+  <conditionalFormatting sqref="DR16:DV267">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK(DR16)), ROUND(DR16, 0) &lt;&gt; ROUND($DQ16, 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DY16:EC267">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>AND(NOT(ISBLANK(DY16)), ROUND(DY16, 0) &lt;&gt; ROUND($DX16, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>